<commit_message>
updated xls files of spark and datasets
</commit_message>
<xml_diff>
--- a/results_analysis/spark_motorFailure_02_hold_01.xlsx
+++ b/results_analysis/spark_motorFailure_02_hold_01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0E030C-4F7E-46EE-9344-6EA415BAD254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8C5B24-0AEE-438D-8D61-0B0BF3B5E34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="734" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="734" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_best" sheetId="11" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="34">
   <si>
     <t>Sparsiciation Method</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>ACC - MEAN - DM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comparison - </t>
   </si>
 </sst>
 </file>
@@ -1043,21 +1046,21 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
         <v>14</v>
       </c>
@@ -1072,8 +1075,8 @@
       <c r="J1" s="70"/>
       <c r="K1" s="70"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1108,7 +1111,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -1143,7 +1146,7 @@
         <v>0.94736842105263197</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -1173,7 +1176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1">
         <v>2</v>
@@ -1206,7 +1209,7 @@
         <v>0.92763157894736903</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
@@ -1237,7 +1240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1272,7 +1275,7 @@
         <v>0.85526315789473695</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -1302,7 +1305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1">
         <v>2</v>
@@ -1335,7 +1338,7 @@
         <v>0.89473684210526305</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
@@ -1366,7 +1369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -1401,7 +1404,7 @@
         <v>0.94078947368421095</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -1431,7 +1434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1">
         <v>2</v>
@@ -1464,7 +1467,7 @@
         <v>0.93421052631579005</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
@@ -1495,7 +1498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -1530,7 +1533,7 @@
         <v>0.96710526315789502</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -1560,7 +1563,7 @@
         <v>0.97368421052631604</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -1593,7 +1596,7 @@
         <v>0.96710526315789502</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
@@ -1624,7 +1627,7 @@
         <v>0.98684210526315796</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
@@ -1634,7 +1637,7 @@
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
@@ -1645,7 +1648,7 @@
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
@@ -1655,7 +1658,7 @@
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
@@ -1665,7 +1668,7 @@
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
@@ -1675,7 +1678,7 @@
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
@@ -1685,7 +1688,7 @@
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
@@ -1695,7 +1698,7 @@
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
@@ -1705,7 +1708,7 @@
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
@@ -1715,7 +1718,7 @@
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
@@ -1725,7 +1728,7 @@
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
@@ -1735,7 +1738,7 @@
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
@@ -1745,7 +1748,7 @@
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
     </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
@@ -1755,7 +1758,7 @@
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
     </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
@@ -1765,7 +1768,7 @@
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
     </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
@@ -1775,7 +1778,7 @@
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
     </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
@@ -1785,7 +1788,7 @@
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
     </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -1795,7 +1798,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -1805,7 +1808,7 @@
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -1815,7 +1818,7 @@
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -1825,7 +1828,7 @@
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -1835,7 +1838,7 @@
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -1845,7 +1848,7 @@
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -1855,7 +1858,7 @@
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -1865,7 +1868,7 @@
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -1875,7 +1878,7 @@
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -1885,7 +1888,7 @@
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
     </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
@@ -1895,7 +1898,7 @@
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
     </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -1905,7 +1908,7 @@
       <c r="J48" s="10"/>
       <c r="K48" s="10"/>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
@@ -1915,7 +1918,7 @@
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
@@ -1925,7 +1928,7 @@
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
@@ -1935,7 +1938,7 @@
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
@@ -1945,7 +1948,7 @@
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
@@ -1968,29 +1971,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E093FD04-CF21-4625-BBAE-D18349CAAAA7}">
   <dimension ref="A1:S53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
         <v>21</v>
       </c>
@@ -2012,8 +2015,8 @@
       <c r="Q1" s="70"/>
       <c r="R1" s="70"/>
     </row>
-    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="75" t="s">
         <v>6</v>
       </c>
@@ -2047,7 +2050,7 @@
       </c>
       <c r="S3" s="74"/>
     </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2106,7 +2109,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -2165,7 +2168,7 @@
         <v>1024.001</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -2219,7 +2222,7 @@
         <v>1024.001</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1">
         <v>2</v>
@@ -2276,7 +2279,7 @@
         <v>1024.001</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
@@ -2331,7 +2334,7 @@
         <v>1024.001</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -2390,7 +2393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -2444,7 +2447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1">
         <v>2</v>
@@ -2501,7 +2504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
@@ -2556,7 +2559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -2615,7 +2618,7 @@
         <v>4.8828125E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -2669,7 +2672,7 @@
         <v>16.0009765625</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1">
         <v>2</v>
@@ -2726,7 +2729,7 @@
         <v>1.66015625E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
@@ -2781,7 +2784,7 @@
         <v>128.0009765625</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -2840,7 +2843,7 @@
         <v>16.0009765625</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -2894,7 +2897,7 @@
         <v>128.0009765625</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -2951,7 +2954,7 @@
         <v>128.0009765625</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
@@ -3006,10 +3009,10 @@
         <v>256.0009765625</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
     </row>
-    <row r="37" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -3026,7 +3029,7 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -3043,7 +3046,7 @@
       <c r="Q38" s="10"/>
       <c r="R38" s="10"/>
     </row>
-    <row r="39" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -3060,7 +3063,7 @@
       <c r="Q39" s="10"/>
       <c r="R39" s="10"/>
     </row>
-    <row r="40" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -3077,7 +3080,7 @@
       <c r="Q40" s="10"/>
       <c r="R40" s="10"/>
     </row>
-    <row r="41" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -3094,7 +3097,7 @@
       <c r="Q41" s="10"/>
       <c r="R41" s="10"/>
     </row>
-    <row r="42" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -3111,7 +3114,7 @@
       <c r="Q42" s="10"/>
       <c r="R42" s="10"/>
     </row>
-    <row r="43" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -3128,7 +3131,7 @@
       <c r="Q43" s="10"/>
       <c r="R43" s="10"/>
     </row>
-    <row r="44" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -3145,7 +3148,7 @@
       <c r="Q44" s="10"/>
       <c r="R44" s="10"/>
     </row>
-    <row r="45" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -3162,7 +3165,7 @@
       <c r="Q45" s="10"/>
       <c r="R45" s="10"/>
     </row>
-    <row r="46" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -3179,7 +3182,7 @@
       <c r="Q46" s="10"/>
       <c r="R46" s="10"/>
     </row>
-    <row r="47" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
@@ -3196,7 +3199,7 @@
       <c r="Q47" s="10"/>
       <c r="R47" s="10"/>
     </row>
-    <row r="48" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -3213,7 +3216,7 @@
       <c r="Q48" s="10"/>
       <c r="R48" s="10"/>
     </row>
-    <row r="49" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
@@ -3230,7 +3233,7 @@
       <c r="Q49" s="10"/>
       <c r="R49" s="10"/>
     </row>
-    <row r="50" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
@@ -3247,7 +3250,7 @@
       <c r="Q50" s="10"/>
       <c r="R50" s="10"/>
     </row>
-    <row r="51" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
@@ -3264,7 +3267,7 @@
       <c r="Q51" s="10"/>
       <c r="R51" s="10"/>
     </row>
-    <row r="52" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
@@ -3281,7 +3284,7 @@
       <c r="Q52" s="10"/>
       <c r="R52" s="10"/>
     </row>
-    <row r="53" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
@@ -3322,17 +3325,17 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -3340,7 +3343,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -3408,7 +3411,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -3444,7 +3447,7 @@
       <c r="V4" s="23"/>
       <c r="W4" s="24"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
@@ -3472,7 +3475,7 @@
       <c r="V5" s="25"/>
       <c r="W5" s="25"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1">
         <v>2</v>
@@ -3504,7 +3507,7 @@
       <c r="V6" s="26"/>
       <c r="W6" s="27"/>
     </row>
-    <row r="7" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
@@ -3532,7 +3535,7 @@
       <c r="V7" s="29"/>
       <c r="W7" s="30"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -3568,7 +3571,7 @@
       <c r="V8" s="32"/>
       <c r="W8" s="33"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
@@ -3596,7 +3599,7 @@
       <c r="V9" s="26"/>
       <c r="W9" s="27"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1">
         <v>2</v>
@@ -3628,7 +3631,7 @@
       <c r="V10" s="26"/>
       <c r="W10" s="27"/>
     </row>
-    <row r="11" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6" t="s">
@@ -3656,7 +3659,7 @@
       <c r="V11" s="29"/>
       <c r="W11" s="30"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -3692,7 +3695,7 @@
       <c r="V12" s="32"/>
       <c r="W12" s="33"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
@@ -3720,7 +3723,7 @@
       <c r="V13" s="26"/>
       <c r="W13" s="27"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1">
         <v>2</v>
@@ -3752,7 +3755,7 @@
       <c r="V14" s="26"/>
       <c r="W14" s="27"/>
     </row>
-    <row r="15" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6" t="s">
@@ -3780,7 +3783,7 @@
       <c r="V15" s="29"/>
       <c r="W15" s="30"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
@@ -3816,7 +3819,7 @@
       <c r="V16" s="32"/>
       <c r="W16" s="33"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
@@ -3844,7 +3847,7 @@
       <c r="V17" s="26"/>
       <c r="W17" s="27"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1">
         <v>2</v>
@@ -3876,7 +3879,7 @@
       <c r="V18" s="26"/>
       <c r="W18" s="27"/>
     </row>
-    <row r="19" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6" t="s">
@@ -3904,7 +3907,7 @@
       <c r="V19" s="29"/>
       <c r="W19" s="30"/>
     </row>
-    <row r="21" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -3912,7 +3915,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -3980,7 +3983,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
@@ -4016,7 +4019,7 @@
       <c r="V23" s="23"/>
       <c r="W23" s="24"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
@@ -4044,7 +4047,7 @@
       <c r="V24" s="26"/>
       <c r="W24" s="27"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1">
         <v>2</v>
@@ -4076,7 +4079,7 @@
       <c r="V25" s="26"/>
       <c r="W25" s="27"/>
     </row>
-    <row r="26" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6" t="s">
@@ -4104,7 +4107,7 @@
       <c r="V26" s="29"/>
       <c r="W26" s="30"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>3</v>
       </c>
@@ -4140,7 +4143,7 @@
       <c r="V27" s="32"/>
       <c r="W27" s="33"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
@@ -4168,7 +4171,7 @@
       <c r="V28" s="26"/>
       <c r="W28" s="27"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1">
         <v>2</v>
@@ -4200,7 +4203,7 @@
       <c r="V29" s="26"/>
       <c r="W29" s="27"/>
     </row>
-    <row r="30" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6" t="s">
@@ -4228,7 +4231,7 @@
       <c r="V30" s="29"/>
       <c r="W30" s="30"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>4</v>
       </c>
@@ -4264,7 +4267,7 @@
       <c r="V31" s="32"/>
       <c r="W31" s="33"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
@@ -4292,7 +4295,7 @@
       <c r="V32" s="26"/>
       <c r="W32" s="27"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="1">
         <v>2</v>
@@ -4324,7 +4327,7 @@
       <c r="V33" s="26"/>
       <c r="W33" s="27"/>
     </row>
-    <row r="34" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6" t="s">
@@ -4352,7 +4355,7 @@
       <c r="V34" s="29"/>
       <c r="W34" s="30"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>5</v>
       </c>
@@ -4388,7 +4391,7 @@
       <c r="V35" s="32"/>
       <c r="W35" s="33"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
@@ -4416,7 +4419,7 @@
       <c r="V36" s="26"/>
       <c r="W36" s="27"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="1">
         <v>2</v>
@@ -4448,7 +4451,7 @@
       <c r="V37" s="26"/>
       <c r="W37" s="27"/>
     </row>
-    <row r="38" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6" t="s">
@@ -4488,27 +4491,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.28515625" customWidth="1"/>
+    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
         <v>14</v>
       </c>
@@ -4523,8 +4530,12 @@
       <c r="J1" s="70"/>
       <c r="K1" s="70"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -4558,8 +4569,41 @@
       <c r="K4" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="S4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="T4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="U4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="V4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="W4" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -4593,8 +4637,25 @@
       <c r="K5" s="24">
         <v>0.81315789473684197</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" s="3">
+        <v>1</v>
+      </c>
+      <c r="O5" s="3">
+        <v>1</v>
+      </c>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="24"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -4623,8 +4684,21 @@
       <c r="K6" s="27">
         <v>0.89210526315789496</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M6" s="4"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26"/>
+      <c r="W6" s="27"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1">
         <v>2</v>
@@ -4656,8 +4730,23 @@
       <c r="K7" s="27">
         <v>0.82828947368421102</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M7" s="4"/>
+      <c r="N7" s="1">
+        <v>2</v>
+      </c>
+      <c r="O7" s="1">
+        <v>1</v>
+      </c>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="26"/>
+      <c r="V7" s="26"/>
+      <c r="W7" s="27"/>
+    </row>
+    <row r="8" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
@@ -4687,8 +4776,21 @@
       <c r="K8" s="30">
         <v>0.88552631578947405</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M8" s="5"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="29"/>
+      <c r="U8" s="29"/>
+      <c r="V8" s="29"/>
+      <c r="W8" s="30"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -4722,8 +4824,25 @@
       <c r="K9" s="33">
         <v>0.740789473684211</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" s="3">
+        <v>1</v>
+      </c>
+      <c r="O9" s="3">
+        <v>1</v>
+      </c>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="32"/>
+      <c r="T9" s="32"/>
+      <c r="U9" s="32"/>
+      <c r="V9" s="32"/>
+      <c r="W9" s="33"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -4752,8 +4871,21 @@
       <c r="K10" s="27">
         <v>0.98355263157894801</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M10" s="4"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="26"/>
+      <c r="R10" s="26"/>
+      <c r="S10" s="26"/>
+      <c r="T10" s="26"/>
+      <c r="U10" s="26"/>
+      <c r="V10" s="26"/>
+      <c r="W10" s="27"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1">
         <v>2</v>
@@ -4785,8 +4917,23 @@
       <c r="K11" s="27">
         <v>0.81842105263157905</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M11" s="4"/>
+      <c r="N11" s="1">
+        <v>2</v>
+      </c>
+      <c r="O11" s="1">
+        <v>1</v>
+      </c>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="26"/>
+      <c r="T11" s="26"/>
+      <c r="U11" s="26"/>
+      <c r="V11" s="26"/>
+      <c r="W11" s="27"/>
+    </row>
+    <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
@@ -4816,8 +4963,21 @@
       <c r="K12" s="30">
         <v>0.90855263157894695</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M12" s="5"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="29"/>
+      <c r="T12" s="29"/>
+      <c r="U12" s="29"/>
+      <c r="V12" s="29"/>
+      <c r="W12" s="30"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -4851,8 +5011,25 @@
       <c r="K13" s="33">
         <v>0.89210526315789496</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N13" s="3">
+        <v>1</v>
+      </c>
+      <c r="O13" s="3">
+        <v>1</v>
+      </c>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="32"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="32"/>
+      <c r="T13" s="32"/>
+      <c r="U13" s="32"/>
+      <c r="V13" s="32"/>
+      <c r="W13" s="33"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -4881,8 +5058,21 @@
       <c r="K14" s="27">
         <v>0.95460526315789496</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M14" s="4"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="26"/>
+      <c r="R14" s="26"/>
+      <c r="S14" s="26"/>
+      <c r="T14" s="26"/>
+      <c r="U14" s="26"/>
+      <c r="V14" s="26"/>
+      <c r="W14" s="27"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1">
         <v>2</v>
@@ -4914,8 +5104,23 @@
       <c r="K15" s="27">
         <v>0.90526315789473699</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M15" s="4"/>
+      <c r="N15" s="1">
+        <v>2</v>
+      </c>
+      <c r="O15" s="1">
+        <v>1</v>
+      </c>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="26"/>
+      <c r="R15" s="26"/>
+      <c r="S15" s="26"/>
+      <c r="T15" s="26"/>
+      <c r="U15" s="26"/>
+      <c r="V15" s="26"/>
+      <c r="W15" s="27"/>
+    </row>
+    <row r="16" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
@@ -4945,8 +5150,21 @@
       <c r="K16" s="30">
         <v>0.96118421052631597</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M16" s="5"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="29"/>
+      <c r="R16" s="29"/>
+      <c r="S16" s="29"/>
+      <c r="T16" s="29"/>
+      <c r="U16" s="29"/>
+      <c r="V16" s="29"/>
+      <c r="W16" s="30"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -4980,8 +5198,25 @@
       <c r="K17" s="33">
         <v>0.91052631578947396</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N17" s="1">
+        <v>1</v>
+      </c>
+      <c r="O17" s="1">
+        <v>1</v>
+      </c>
+      <c r="P17" s="31"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="32"/>
+      <c r="T17" s="32"/>
+      <c r="U17" s="32"/>
+      <c r="V17" s="32"/>
+      <c r="W17" s="33"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -5010,8 +5245,21 @@
       <c r="K18" s="27">
         <v>0.92894736842105297</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M18" s="4"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="26"/>
+      <c r="R18" s="26"/>
+      <c r="S18" s="26"/>
+      <c r="T18" s="26"/>
+      <c r="U18" s="26"/>
+      <c r="V18" s="26"/>
+      <c r="W18" s="27"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -5043,8 +5291,23 @@
       <c r="K19" s="27">
         <v>0.86250000000000004</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M19" s="4"/>
+      <c r="N19" s="1">
+        <v>2</v>
+      </c>
+      <c r="O19" s="1">
+        <v>1</v>
+      </c>
+      <c r="P19" s="25"/>
+      <c r="Q19" s="26"/>
+      <c r="R19" s="26"/>
+      <c r="S19" s="26"/>
+      <c r="T19" s="26"/>
+      <c r="U19" s="26"/>
+      <c r="V19" s="26"/>
+      <c r="W19" s="27"/>
+    </row>
+    <row r="20" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
@@ -5074,8 +5337,21 @@
       <c r="K20" s="30">
         <v>0.90789473684210498</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M20" s="5"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="29"/>
+      <c r="S20" s="29"/>
+      <c r="T20" s="29"/>
+      <c r="U20" s="29"/>
+      <c r="V20" s="29"/>
+      <c r="W20" s="30"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
@@ -5085,7 +5361,7 @@
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
@@ -5096,7 +5372,7 @@
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
@@ -5106,7 +5382,7 @@
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
@@ -5116,7 +5392,7 @@
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
@@ -5126,7 +5402,7 @@
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
@@ -5136,7 +5412,7 @@
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
@@ -5146,7 +5422,7 @@
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
@@ -5156,7 +5432,7 @@
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
@@ -5166,7 +5442,7 @@
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
@@ -5176,7 +5452,7 @@
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
@@ -5186,7 +5462,7 @@
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
@@ -5196,7 +5472,7 @@
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
     </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
@@ -5206,7 +5482,7 @@
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
     </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
@@ -5216,7 +5492,7 @@
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
     </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
@@ -5226,7 +5502,7 @@
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
     </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
@@ -5236,7 +5512,7 @@
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
     </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -5246,7 +5522,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -5256,7 +5532,7 @@
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -5266,7 +5542,7 @@
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -5276,7 +5552,7 @@
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -5286,7 +5562,7 @@
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -5296,7 +5572,7 @@
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -5306,7 +5582,7 @@
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -5316,7 +5592,7 @@
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -5326,7 +5602,7 @@
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -5336,7 +5612,7 @@
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
     </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
@@ -5346,7 +5622,7 @@
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
     </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -5356,7 +5632,7 @@
       <c r="J48" s="10"/>
       <c r="K48" s="10"/>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
@@ -5366,7 +5642,7 @@
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
@@ -5376,7 +5652,7 @@
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
@@ -5386,7 +5662,7 @@
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
@@ -5396,7 +5672,7 @@
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
@@ -5422,21 +5698,21 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
         <v>14</v>
       </c>
@@ -5451,8 +5727,8 @@
       <c r="J1" s="70"/>
       <c r="K1" s="70"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -5487,7 +5763,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -5522,7 +5798,7 @@
         <v>9.8327816487651695E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -5552,7 +5828,7 @@
         <v>0.12776640253406801</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1">
         <v>2</v>
@@ -5585,7 +5861,7 @@
         <v>7.7250900321565605E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
@@ -5616,7 +5892,7 @@
         <v>0.131586257106899</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -5651,7 +5927,7 @@
         <v>6.9014520220248898E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -5681,7 +5957,7 @@
         <v>1.7612257022159E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1">
         <v>2</v>
@@ -5714,7 +5990,7 @@
         <v>6.4995205448570903E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
@@ -5745,7 +6021,7 @@
         <v>0.110281073646743</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -5780,7 +6056,7 @@
         <v>3.5523608300555398E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -5810,7 +6086,7 @@
         <v>3.59609005036775E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1">
         <v>2</v>
@@ -5843,7 +6119,7 @@
         <v>1.8400155231055301E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
@@ -5874,7 +6150,7 @@
         <v>5.0908376710802901E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -5909,7 +6185,7 @@
         <v>8.5114844654430602E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -5939,7 +6215,7 @@
         <v>3.3373705929380403E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -5972,7 +6248,7 @@
         <v>0.118844677635465</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
@@ -6003,7 +6279,7 @@
         <v>8.0216408588473204E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
@@ -6013,7 +6289,7 @@
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
@@ -6024,7 +6300,7 @@
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
@@ -6034,7 +6310,7 @@
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
@@ -6044,7 +6320,7 @@
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
@@ -6054,7 +6330,7 @@
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
@@ -6064,7 +6340,7 @@
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
@@ -6074,7 +6350,7 @@
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
@@ -6084,7 +6360,7 @@
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
@@ -6094,7 +6370,7 @@
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
@@ -6104,7 +6380,7 @@
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
@@ -6114,7 +6390,7 @@
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
@@ -6124,7 +6400,7 @@
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
     </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
@@ -6134,7 +6410,7 @@
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
     </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
@@ -6144,7 +6420,7 @@
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
     </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
@@ -6154,7 +6430,7 @@
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
     </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
@@ -6164,7 +6440,7 @@
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
     </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -6174,7 +6450,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -6184,7 +6460,7 @@
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -6194,7 +6470,7 @@
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -6204,7 +6480,7 @@
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -6214,7 +6490,7 @@
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -6224,7 +6500,7 @@
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -6234,7 +6510,7 @@
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -6244,7 +6520,7 @@
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -6254,7 +6530,7 @@
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -6264,7 +6540,7 @@
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
     </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
@@ -6274,7 +6550,7 @@
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
     </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -6284,7 +6560,7 @@
       <c r="J48" s="10"/>
       <c r="K48" s="10"/>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
@@ -6294,7 +6570,7 @@
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
@@ -6304,7 +6580,7 @@
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
@@ -6314,7 +6590,7 @@
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
@@ -6324,7 +6600,7 @@
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
@@ -6350,21 +6626,21 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
         <v>13</v>
       </c>
@@ -6379,8 +6655,8 @@
       <c r="J1" s="70"/>
       <c r="K1" s="70"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -6415,7 +6691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -6450,7 +6726,7 @@
         <v>0.77960526315789502</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -6480,7 +6756,7 @@
         <v>0.95065789473684204</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1">
         <v>2</v>
@@ -6513,7 +6789,7 @@
         <v>0.83223684210526305</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
@@ -6544,7 +6820,7 @@
         <v>0.95723684210526305</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -6579,7 +6855,7 @@
         <v>0.73026315789473695</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -6609,7 +6885,7 @@
         <v>0.98684210526315796</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1">
         <v>2</v>
@@ -6642,7 +6918,7 @@
         <v>0.83552631578947401</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
@@ -6673,7 +6949,7 @@
         <v>0.98684210526315796</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -6708,7 +6984,7 @@
         <v>0.89473684210526305</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -6738,7 +7014,7 @@
         <v>0.94407894736842102</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1">
         <v>2</v>
@@ -6771,7 +7047,7 @@
         <v>0.90131578947368396</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
@@ -6802,7 +7078,7 @@
         <v>0.98026315789473695</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -6837,7 +7113,7 @@
         <v>0.94078947368421095</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -6867,7 +7143,7 @@
         <v>0.93421052631579005</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -6900,7 +7176,7 @@
         <v>0.92434210526315796</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
@@ -6931,10 +7207,10 @@
         <v>0.92105263157894701</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
     </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -6944,7 +7220,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -6954,7 +7230,7 @@
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -6964,7 +7240,7 @@
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -6974,7 +7250,7 @@
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -6984,7 +7260,7 @@
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -6994,7 +7270,7 @@
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -7004,7 +7280,7 @@
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -7014,7 +7290,7 @@
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -7024,7 +7300,7 @@
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -7034,7 +7310,7 @@
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
     </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
@@ -7044,7 +7320,7 @@
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
     </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -7054,7 +7330,7 @@
       <c r="J48" s="10"/>
       <c r="K48" s="10"/>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
@@ -7064,7 +7340,7 @@
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
@@ -7074,7 +7350,7 @@
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
@@ -7084,7 +7360,7 @@
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
@@ -7094,7 +7370,7 @@
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
@@ -7120,21 +7396,21 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.33203125" customWidth="1"/>
-    <col min="10" max="10" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
         <v>18</v>
       </c>
@@ -7149,8 +7425,8 @@
       <c r="J1" s="70"/>
       <c r="K1" s="70"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -7185,7 +7461,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -7220,7 +7496,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -7250,7 +7526,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1">
         <v>2</v>
@@ -7283,7 +7559,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
@@ -7314,7 +7590,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -7349,7 +7625,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -7379,7 +7655,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1">
         <v>2</v>
@@ -7412,7 +7688,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
@@ -7443,7 +7719,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -7478,7 +7754,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -7508,7 +7784,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1">
         <v>2</v>
@@ -7541,7 +7817,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
@@ -7572,7 +7848,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -7607,7 +7883,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -7637,7 +7913,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -7670,7 +7946,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
@@ -7701,10 +7977,10 @@
         <v>140</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
     </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -7714,7 +7990,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -7724,7 +8000,7 @@
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -7734,7 +8010,7 @@
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -7744,7 +8020,7 @@
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -7754,7 +8030,7 @@
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -7764,7 +8040,7 @@
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -7774,7 +8050,7 @@
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -7784,7 +8060,7 @@
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -7794,7 +8070,7 @@
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -7804,7 +8080,7 @@
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
     </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
@@ -7814,7 +8090,7 @@
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
     </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -7824,7 +8100,7 @@
       <c r="J48" s="10"/>
       <c r="K48" s="10"/>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
@@ -7834,7 +8110,7 @@
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
@@ -7844,7 +8120,7 @@
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
@@ -7854,7 +8130,7 @@
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
@@ -7864,7 +8140,7 @@
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
@@ -7890,22 +8166,22 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.44140625" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
         <v>19</v>
       </c>
@@ -7920,8 +8196,8 @@
       <c r="J1" s="70"/>
       <c r="K1" s="70"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -7956,7 +8232,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -7991,7 +8267,7 @@
         <v>106.6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -8021,7 +8297,7 @@
         <v>160.9</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1">
         <v>2</v>
@@ -8054,7 +8330,7 @@
         <v>96.7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
@@ -8085,7 +8361,7 @@
         <v>158.9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -8120,7 +8396,7 @@
         <v>50.9</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -8150,7 +8426,7 @@
         <v>220.3</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1">
         <v>2</v>
@@ -8183,7 +8459,7 @@
         <v>95.2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
@@ -8214,7 +8490,7 @@
         <v>163.1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -8249,7 +8525,7 @@
         <v>70.099999999999994</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -8279,7 +8555,7 @@
         <v>61.6</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1">
         <v>2</v>
@@ -8312,7 +8588,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
@@ -8343,7 +8619,7 @@
         <v>53.5</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -8378,7 +8654,7 @@
         <v>193.1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -8408,7 +8684,7 @@
         <v>130.5</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -8441,7 +8717,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
@@ -8472,10 +8748,10 @@
         <v>108.3</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
     </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -8485,7 +8761,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -8495,7 +8771,7 @@
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -8505,7 +8781,7 @@
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -8515,7 +8791,7 @@
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -8525,7 +8801,7 @@
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -8535,7 +8811,7 @@
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -8545,7 +8821,7 @@
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -8555,7 +8831,7 @@
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -8565,7 +8841,7 @@
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -8575,7 +8851,7 @@
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
     </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
@@ -8585,7 +8861,7 @@
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
     </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -8595,7 +8871,7 @@
       <c r="J48" s="10"/>
       <c r="K48" s="10"/>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
@@ -8605,7 +8881,7 @@
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
@@ -8615,7 +8891,7 @@
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
@@ -8625,7 +8901,7 @@
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
@@ -8635,7 +8911,7 @@
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
@@ -8661,21 +8937,21 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
         <v>20</v>
       </c>
@@ -8690,8 +8966,8 @@
       <c r="J1" s="70"/>
       <c r="K1" s="70"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -8726,7 +9002,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -8761,7 +9037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -8791,7 +9067,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1">
         <v>2</v>
@@ -8824,7 +9100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
@@ -8855,7 +9131,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -8890,7 +9166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -8920,7 +9196,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1">
         <v>2</v>
@@ -8953,7 +9229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
@@ -8984,7 +9260,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -9019,7 +9295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -9049,7 +9325,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1">
         <v>2</v>
@@ -9082,7 +9358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
@@ -9113,7 +9389,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -9148,7 +9424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -9178,7 +9454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -9211,7 +9487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
@@ -9242,10 +9518,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
     </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -9255,7 +9531,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -9265,7 +9541,7 @@
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -9275,7 +9551,7 @@
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -9285,7 +9561,7 @@
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -9295,7 +9571,7 @@
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -9305,7 +9581,7 @@
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -9315,7 +9591,7 @@
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -9325,7 +9601,7 @@
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -9335,7 +9611,7 @@
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -9345,7 +9621,7 @@
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
     </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
@@ -9355,7 +9631,7 @@
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
     </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -9365,7 +9641,7 @@
       <c r="J48" s="10"/>
       <c r="K48" s="10"/>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
@@ -9375,7 +9651,7 @@
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
@@ -9385,7 +9661,7 @@
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
@@ -9395,7 +9671,7 @@
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
@@ -9405,7 +9681,7 @@
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
@@ -9431,21 +9707,21 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
         <v>21</v>
       </c>
@@ -9460,8 +9736,8 @@
       <c r="J1" s="70"/>
       <c r="K1" s="70"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -9496,7 +9772,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -9531,7 +9807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -9561,7 +9837,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1">
         <v>2</v>
@@ -9594,7 +9870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
@@ -9625,7 +9901,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -9660,7 +9936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -9690,7 +9966,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1">
         <v>2</v>
@@ -9723,7 +9999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
@@ -9754,7 +10030,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -9789,7 +10065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -9819,7 +10095,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1">
         <v>2</v>
@@ -9852,7 +10128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
@@ -9883,7 +10159,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -9918,7 +10194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -9948,7 +10224,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -9981,7 +10257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
@@ -10012,10 +10288,10 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
     </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -10025,7 +10301,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -10035,7 +10311,7 @@
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -10045,7 +10321,7 @@
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -10055,7 +10331,7 @@
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -10065,7 +10341,7 @@
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -10075,7 +10351,7 @@
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -10085,7 +10361,7 @@
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -10095,7 +10371,7 @@
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -10105,7 +10381,7 @@
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -10115,7 +10391,7 @@
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
     </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
@@ -10125,7 +10401,7 @@
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
     </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -10135,7 +10411,7 @@
       <c r="J48" s="10"/>
       <c r="K48" s="10"/>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
@@ -10145,7 +10421,7 @@
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
@@ -10155,7 +10431,7 @@
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
@@ -10165,7 +10441,7 @@
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
@@ -10175,7 +10451,7 @@
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
@@ -10201,26 +10477,26 @@
       <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.44140625" customWidth="1"/>
-    <col min="15" max="15" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.42578125" customWidth="1"/>
+    <col min="15" max="15" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
         <v>26</v>
       </c>
@@ -10240,8 +10516,8 @@
       <c r="O1" s="70"/>
       <c r="P1" s="70"/>
     </row>
-    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="13" t="s">
         <v>6</v>
       </c>
@@ -10272,7 +10548,7 @@
       </c>
       <c r="P3" s="74"/>
     </row>
-    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -10322,7 +10598,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -10372,7 +10648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="17" t="s">
         <v>12</v>
@@ -10417,7 +10693,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1">
         <v>2</v>
@@ -10465,7 +10741,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="18" t="s">
@@ -10511,7 +10787,7 @@
         <v>1.5625E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -10561,7 +10837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="17" t="s">
         <v>12</v>
@@ -10606,7 +10882,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1">
         <v>2</v>
@@ -10654,7 +10930,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="18" t="s">
@@ -10700,7 +10976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -10750,7 +11026,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="17" t="s">
         <v>12</v>
@@ -10795,7 +11071,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1">
         <v>2</v>
@@ -10843,7 +11119,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="18" t="s">
@@ -10889,7 +11165,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -10939,7 +11215,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="17" t="s">
         <v>12</v>
@@ -10984,7 +11260,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -11032,7 +11308,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="18" t="s">
@@ -11078,10 +11354,10 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
     </row>
-    <row r="37" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -11095,7 +11371,7 @@
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
     </row>
-    <row r="38" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -11109,7 +11385,7 @@
       <c r="N38" s="10"/>
       <c r="O38" s="10"/>
     </row>
-    <row r="39" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -11123,7 +11399,7 @@
       <c r="N39" s="10"/>
       <c r="O39" s="10"/>
     </row>
-    <row r="40" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -11137,7 +11413,7 @@
       <c r="N40" s="10"/>
       <c r="O40" s="10"/>
     </row>
-    <row r="41" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -11151,7 +11427,7 @@
       <c r="N41" s="10"/>
       <c r="O41" s="10"/>
     </row>
-    <row r="42" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -11165,7 +11441,7 @@
       <c r="N42" s="10"/>
       <c r="O42" s="10"/>
     </row>
-    <row r="43" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -11179,7 +11455,7 @@
       <c r="N43" s="10"/>
       <c r="O43" s="10"/>
     </row>
-    <row r="44" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -11193,7 +11469,7 @@
       <c r="N44" s="10"/>
       <c r="O44" s="10"/>
     </row>
-    <row r="45" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -11207,7 +11483,7 @@
       <c r="N45" s="10"/>
       <c r="O45" s="10"/>
     </row>
-    <row r="46" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -11221,7 +11497,7 @@
       <c r="N46" s="10"/>
       <c r="O46" s="10"/>
     </row>
-    <row r="47" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
@@ -11235,7 +11511,7 @@
       <c r="N47" s="10"/>
       <c r="O47" s="10"/>
     </row>
-    <row r="48" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -11249,7 +11525,7 @@
       <c r="N48" s="10"/>
       <c r="O48" s="10"/>
     </row>
-    <row r="49" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
@@ -11263,7 +11539,7 @@
       <c r="N49" s="10"/>
       <c r="O49" s="10"/>
     </row>
-    <row r="50" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
@@ -11277,7 +11553,7 @@
       <c r="N50" s="10"/>
       <c r="O50" s="10"/>
     </row>
-    <row r="51" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
@@ -11291,7 +11567,7 @@
       <c r="N51" s="10"/>
       <c r="O51" s="10"/>
     </row>
-    <row r="52" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
@@ -11305,7 +11581,7 @@
       <c r="N52" s="10"/>
       <c r="O52" s="10"/>
     </row>
-    <row r="53" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>

</xml_diff>

<commit_message>
fixing some errors in results matrices
</commit_message>
<xml_diff>
--- a/results_analysis/spark_motorFailure_02_hold_01.xlsx
+++ b/results_analysis/spark_motorFailure_02_hold_01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55F811C-1509-4DEB-8232-860EA0B984B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD3BF49-C3F8-4C9B-AD69-659A455E2DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="734" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="734" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_best" sheetId="11" r:id="rId1"/>
@@ -152,8 +152,16 @@
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -528,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -753,6 +761,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4496,8 +4531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4625,19 +4660,19 @@
       <c r="F5" s="23">
         <v>0.77763157894736901</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="76">
         <v>0.79934210526315796</v>
       </c>
       <c r="H5" s="23">
         <v>0.76315789473684204</v>
       </c>
-      <c r="I5" s="23">
+      <c r="I5" s="76">
         <v>0.89078947368421102</v>
       </c>
       <c r="J5" s="23">
         <v>0.66710526315789498</v>
       </c>
-      <c r="K5" s="24">
+      <c r="K5" s="77">
         <v>0.81315789473684197</v>
       </c>
       <c r="M5" s="2" t="s">
@@ -4672,10 +4707,10 @@
       <c r="F6" s="26">
         <v>0.70263157894736905</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="78">
         <v>0.89013157894736905</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H6" s="78">
         <v>0.87828947368420995</v>
       </c>
       <c r="I6" s="26">
@@ -4684,7 +4719,7 @@
       <c r="J6" s="26">
         <v>0.63421052631579</v>
       </c>
-      <c r="K6" s="27">
+      <c r="K6" s="79">
         <v>0.89210526315789496</v>
       </c>
       <c r="M6" s="4"/>
@@ -4715,7 +4750,7 @@
       <c r="E7" s="26">
         <v>0.78223684210526301</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="78">
         <v>0.80197368421052595</v>
       </c>
       <c r="G7" s="26">
@@ -4724,13 +4759,13 @@
       <c r="H7" s="26">
         <v>0.77368421052631597</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="78">
         <v>0.80657894736842095</v>
       </c>
       <c r="J7" s="26">
         <v>0.69407894736842102</v>
       </c>
-      <c r="K7" s="27">
+      <c r="K7" s="79">
         <v>0.82828947368421102</v>
       </c>
       <c r="M7" s="4"/>
@@ -4764,10 +4799,10 @@
       <c r="F8" s="29">
         <v>0.78815789473684195</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="81">
         <v>0.84210526315789502</v>
       </c>
-      <c r="H8" s="29">
+      <c r="H8" s="81">
         <v>0.84276315789473699</v>
       </c>
       <c r="I8" s="29">
@@ -4776,7 +4811,7 @@
       <c r="J8" s="29">
         <v>0.68223684210526303</v>
       </c>
-      <c r="K8" s="30">
+      <c r="K8" s="80">
         <v>0.88552631578947405</v>
       </c>
       <c r="M8" s="5"/>
@@ -4806,10 +4841,10 @@
       <c r="D9" s="31">
         <v>0.77500000000000002</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="82">
         <v>0.80197368421052595</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="82">
         <v>0.83881578947368396</v>
       </c>
       <c r="G9" s="32">
@@ -4818,7 +4853,7 @@
       <c r="H9" s="32">
         <v>0.78947368421052599</v>
       </c>
-      <c r="I9" s="32">
+      <c r="I9" s="82">
         <v>0.91973684210526296</v>
       </c>
       <c r="J9" s="32">
@@ -4862,16 +4897,16 @@
       <c r="G10" s="26">
         <v>0.87368421052631595</v>
       </c>
-      <c r="H10" s="26">
+      <c r="H10" s="78">
         <v>0.96644736842105305</v>
       </c>
-      <c r="I10" s="26">
+      <c r="I10" s="78">
         <v>0.92236842105263195</v>
       </c>
       <c r="J10" s="26">
         <v>0.75855263157894703</v>
       </c>
-      <c r="K10" s="27">
+      <c r="K10" s="79">
         <v>0.98355263157894801</v>
       </c>
       <c r="M10" s="4"/>
@@ -4902,7 +4937,7 @@
       <c r="E11" s="26">
         <v>0.76973684210526305</v>
       </c>
-      <c r="F11" s="26">
+      <c r="F11" s="78">
         <v>0.85</v>
       </c>
       <c r="G11" s="26">
@@ -4911,13 +4946,13 @@
       <c r="H11" s="26">
         <v>0.77171052631578896</v>
       </c>
-      <c r="I11" s="26">
+      <c r="I11" s="78">
         <v>0.91513157894736896</v>
       </c>
-      <c r="J11" s="26">
+      <c r="J11" s="78">
         <v>0.86315789473684201</v>
       </c>
-      <c r="K11" s="27">
+      <c r="K11" s="83">
         <v>0.81842105263157905</v>
       </c>
       <c r="M11" s="4"/>
@@ -4954,16 +4989,16 @@
       <c r="G12" s="29">
         <v>0.83947368421052604</v>
       </c>
-      <c r="H12" s="29">
+      <c r="H12" s="81">
         <v>0.932894736842105</v>
       </c>
-      <c r="I12" s="29">
+      <c r="I12" s="81">
         <v>0.92171052631578898</v>
       </c>
       <c r="J12" s="29">
         <v>0.70065789473684204</v>
       </c>
-      <c r="K12" s="30">
+      <c r="K12" s="80">
         <v>0.90855263157894695</v>
       </c>
       <c r="M12" s="5"/>
@@ -4993,13 +5028,13 @@
       <c r="D13" s="31">
         <v>0.89473684210526305</v>
       </c>
-      <c r="E13" s="32">
+      <c r="E13" s="82">
         <v>0.90263157894736801</v>
       </c>
       <c r="F13" s="32">
         <v>0.893421052631579</v>
       </c>
-      <c r="G13" s="32">
+      <c r="G13" s="82">
         <v>0.89605263157894699</v>
       </c>
       <c r="H13" s="32">
@@ -5011,7 +5046,7 @@
       <c r="J13" s="32">
         <v>0.85</v>
       </c>
-      <c r="K13" s="33">
+      <c r="K13" s="84">
         <v>0.89210526315789496</v>
       </c>
       <c r="M13" s="2" t="s">
@@ -5040,13 +5075,13 @@
       <c r="D14" s="25">
         <v>0.88552631578947405</v>
       </c>
-      <c r="E14" s="26">
+      <c r="E14" s="78">
         <v>0.99736842105263201</v>
       </c>
       <c r="F14" s="26">
         <v>0.89144736842105299</v>
       </c>
-      <c r="G14" s="26">
+      <c r="G14" s="78">
         <v>0.99868421052631595</v>
       </c>
       <c r="H14" s="26">
@@ -5058,7 +5093,7 @@
       <c r="J14" s="26">
         <v>0.78486842105263199</v>
       </c>
-      <c r="K14" s="27">
+      <c r="K14" s="79">
         <v>0.95460526315789496</v>
       </c>
       <c r="M14" s="4"/>
@@ -5095,16 +5130,16 @@
       <c r="G15" s="26">
         <v>0.856578947368421</v>
       </c>
-      <c r="H15" s="26">
+      <c r="H15" s="78">
         <v>0.88289473684210495</v>
       </c>
-      <c r="I15" s="26">
+      <c r="I15" s="78">
         <v>0.88026315789473697</v>
       </c>
       <c r="J15" s="26">
         <v>0.84473684210526301</v>
       </c>
-      <c r="K15" s="27">
+      <c r="K15" s="79">
         <v>0.90526315789473699</v>
       </c>
       <c r="M15" s="4"/>
@@ -5132,13 +5167,13 @@
       <c r="D16" s="28">
         <v>0.875</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="81">
         <v>0.99868421052631595</v>
       </c>
       <c r="F16" s="29">
         <v>0.88355263157894703</v>
       </c>
-      <c r="G16" s="29">
+      <c r="G16" s="81">
         <v>0.99342105263157898</v>
       </c>
       <c r="H16" s="29">
@@ -5150,7 +5185,7 @@
       <c r="J16" s="29">
         <v>0.81118421052631595</v>
       </c>
-      <c r="K16" s="30">
+      <c r="K16" s="80">
         <v>0.96118421052631597</v>
       </c>
       <c r="M16" s="5"/>
@@ -5186,10 +5221,10 @@
       <c r="F17" s="32">
         <v>0.76644736842105299</v>
       </c>
-      <c r="G17" s="32">
+      <c r="G17" s="82">
         <v>0.91447368421052599</v>
       </c>
-      <c r="H17" s="32">
+      <c r="H17" s="82">
         <v>0.84802631578947396</v>
       </c>
       <c r="I17" s="32">
@@ -5198,7 +5233,7 @@
       <c r="J17" s="32">
         <v>0.68552631578947398</v>
       </c>
-      <c r="K17" s="33">
+      <c r="K17" s="84">
         <v>0.91052631578947396</v>
       </c>
       <c r="M17" s="4" t="s">
@@ -5227,7 +5262,7 @@
       <c r="D18" s="25">
         <v>0.66315789473684195</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E18" s="78">
         <v>0.93355263157894697</v>
       </c>
       <c r="F18" s="26">
@@ -5236,7 +5271,7 @@
       <c r="G18" s="26">
         <v>0.92631578947368398</v>
       </c>
-      <c r="H18" s="26">
+      <c r="H18" s="78">
         <v>0.93552631578947398</v>
       </c>
       <c r="I18" s="26">
@@ -5245,7 +5280,7 @@
       <c r="J18" s="26">
         <v>0.61776315789473701</v>
       </c>
-      <c r="K18" s="27">
+      <c r="K18" s="79">
         <v>0.92894736842105297</v>
       </c>
       <c r="M18" s="4"/>
@@ -5279,19 +5314,19 @@
       <c r="F19" s="26">
         <v>0.78421052631579002</v>
       </c>
-      <c r="G19" s="26">
+      <c r="G19" s="78">
         <v>0.879605263157895</v>
       </c>
       <c r="H19" s="26">
         <v>0.84934210526315801</v>
       </c>
-      <c r="I19" s="26">
+      <c r="I19" s="78">
         <v>0.88815789473684204</v>
       </c>
       <c r="J19" s="26">
         <v>0.70263157894736905</v>
       </c>
-      <c r="K19" s="27">
+      <c r="K19" s="79">
         <v>0.86250000000000004</v>
       </c>
       <c r="M19" s="4"/>
@@ -5325,10 +5360,10 @@
       <c r="F20" s="29">
         <v>0.71447368421052604</v>
       </c>
-      <c r="G20" s="29">
+      <c r="G20" s="81">
         <v>0.90131578947368396</v>
       </c>
-      <c r="H20" s="29">
+      <c r="H20" s="81">
         <v>0.932894736842105</v>
       </c>
       <c r="I20" s="29">
@@ -5337,7 +5372,7 @@
       <c r="J20" s="29">
         <v>0.69868421052631602</v>
       </c>
-      <c r="K20" s="30">
+      <c r="K20" s="80">
         <v>0.90789473684210498</v>
       </c>
       <c r="M20" s="5"/>
@@ -5697,8 +5732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D83308-7EFF-4F48-ACED-83B85BC27520}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
adding results of spark reduced matrices
</commit_message>
<xml_diff>
--- a/results_analysis/spark_motorFailure_02_hold_01.xlsx
+++ b/results_analysis/spark_motorFailure_02_hold_01.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD3BF49-C3F8-4C9B-AD69-659A455E2DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3288B965-877E-42D7-8DBA-4DFF21591614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="734" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="35">
   <si>
     <t>Sparsiciation Method</t>
   </si>
@@ -536,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -745,24 +745,6 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -784,10 +766,79 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1099,19 +1150,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2032,61 +2083,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="75" t="s">
+      <c r="D3" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="73"/>
-      <c r="F3" s="72" t="s">
+      <c r="E3" s="81"/>
+      <c r="F3" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="73"/>
-      <c r="H3" s="72" t="s">
+      <c r="G3" s="81"/>
+      <c r="H3" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="73"/>
-      <c r="J3" s="72" t="s">
+      <c r="I3" s="81"/>
+      <c r="J3" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="73"/>
-      <c r="L3" s="72" t="s">
+      <c r="K3" s="81"/>
+      <c r="L3" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="73"/>
-      <c r="N3" s="72" t="s">
+      <c r="M3" s="81"/>
+      <c r="N3" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="73"/>
-      <c r="P3" s="72" t="s">
+      <c r="O3" s="81"/>
+      <c r="P3" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="73"/>
-      <c r="R3" s="72" t="s">
+      <c r="Q3" s="81"/>
+      <c r="R3" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="74"/>
+      <c r="S3" s="82"/>
     </row>
     <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
@@ -4529,10 +4580,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W53"/>
+  <dimension ref="A1:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4554,19 +4605,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
     </row>
     <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="M3" t="s">
@@ -4660,19 +4711,19 @@
       <c r="F5" s="23">
         <v>0.77763157894736901</v>
       </c>
-      <c r="G5" s="76">
+      <c r="G5" s="70">
         <v>0.79934210526315796</v>
       </c>
       <c r="H5" s="23">
         <v>0.76315789473684204</v>
       </c>
-      <c r="I5" s="76">
+      <c r="I5" s="70">
         <v>0.89078947368421102</v>
       </c>
       <c r="J5" s="23">
         <v>0.66710526315789498</v>
       </c>
-      <c r="K5" s="77">
+      <c r="K5" s="71">
         <v>0.81315789473684197</v>
       </c>
       <c r="M5" s="2" t="s">
@@ -4707,10 +4758,10 @@
       <c r="F6" s="26">
         <v>0.70263157894736905</v>
       </c>
-      <c r="G6" s="78">
+      <c r="G6" s="72">
         <v>0.89013157894736905</v>
       </c>
-      <c r="H6" s="78">
+      <c r="H6" s="72">
         <v>0.87828947368420995</v>
       </c>
       <c r="I6" s="26">
@@ -4719,7 +4770,7 @@
       <c r="J6" s="26">
         <v>0.63421052631579</v>
       </c>
-      <c r="K6" s="79">
+      <c r="K6" s="73">
         <v>0.89210526315789496</v>
       </c>
       <c r="M6" s="4"/>
@@ -4750,7 +4801,7 @@
       <c r="E7" s="26">
         <v>0.78223684210526301</v>
       </c>
-      <c r="F7" s="78">
+      <c r="F7" s="72">
         <v>0.80197368421052595</v>
       </c>
       <c r="G7" s="26">
@@ -4759,13 +4810,13 @@
       <c r="H7" s="26">
         <v>0.77368421052631597</v>
       </c>
-      <c r="I7" s="78">
+      <c r="I7" s="72">
         <v>0.80657894736842095</v>
       </c>
       <c r="J7" s="26">
         <v>0.69407894736842102</v>
       </c>
-      <c r="K7" s="79">
+      <c r="K7" s="73">
         <v>0.82828947368421102</v>
       </c>
       <c r="M7" s="4"/>
@@ -4799,10 +4850,10 @@
       <c r="F8" s="29">
         <v>0.78815789473684195</v>
       </c>
-      <c r="G8" s="81">
+      <c r="G8" s="75">
         <v>0.84210526315789502</v>
       </c>
-      <c r="H8" s="81">
+      <c r="H8" s="75">
         <v>0.84276315789473699</v>
       </c>
       <c r="I8" s="29">
@@ -4811,7 +4862,7 @@
       <c r="J8" s="29">
         <v>0.68223684210526303</v>
       </c>
-      <c r="K8" s="80">
+      <c r="K8" s="74">
         <v>0.88552631578947405</v>
       </c>
       <c r="M8" s="5"/>
@@ -4841,10 +4892,10 @@
       <c r="D9" s="31">
         <v>0.77500000000000002</v>
       </c>
-      <c r="E9" s="82">
+      <c r="E9" s="76">
         <v>0.80197368421052595</v>
       </c>
-      <c r="F9" s="82">
+      <c r="F9" s="76">
         <v>0.83881578947368396</v>
       </c>
       <c r="G9" s="32">
@@ -4853,7 +4904,7 @@
       <c r="H9" s="32">
         <v>0.78947368421052599</v>
       </c>
-      <c r="I9" s="82">
+      <c r="I9" s="76">
         <v>0.91973684210526296</v>
       </c>
       <c r="J9" s="32">
@@ -4897,16 +4948,16 @@
       <c r="G10" s="26">
         <v>0.87368421052631595</v>
       </c>
-      <c r="H10" s="78">
+      <c r="H10" s="72">
         <v>0.96644736842105305</v>
       </c>
-      <c r="I10" s="78">
+      <c r="I10" s="72">
         <v>0.92236842105263195</v>
       </c>
       <c r="J10" s="26">
         <v>0.75855263157894703</v>
       </c>
-      <c r="K10" s="79">
+      <c r="K10" s="73">
         <v>0.98355263157894801</v>
       </c>
       <c r="M10" s="4"/>
@@ -4937,7 +4988,7 @@
       <c r="E11" s="26">
         <v>0.76973684210526305</v>
       </c>
-      <c r="F11" s="78">
+      <c r="F11" s="72">
         <v>0.85</v>
       </c>
       <c r="G11" s="26">
@@ -4946,13 +4997,13 @@
       <c r="H11" s="26">
         <v>0.77171052631578896</v>
       </c>
-      <c r="I11" s="78">
+      <c r="I11" s="72">
         <v>0.91513157894736896</v>
       </c>
-      <c r="J11" s="78">
+      <c r="J11" s="72">
         <v>0.86315789473684201</v>
       </c>
-      <c r="K11" s="83">
+      <c r="K11" s="27">
         <v>0.81842105263157905</v>
       </c>
       <c r="M11" s="4"/>
@@ -4989,16 +5040,16 @@
       <c r="G12" s="29">
         <v>0.83947368421052604</v>
       </c>
-      <c r="H12" s="81">
+      <c r="H12" s="75">
         <v>0.932894736842105</v>
       </c>
-      <c r="I12" s="81">
+      <c r="I12" s="75">
         <v>0.92171052631578898</v>
       </c>
       <c r="J12" s="29">
         <v>0.70065789473684204</v>
       </c>
-      <c r="K12" s="80">
+      <c r="K12" s="74">
         <v>0.90855263157894695</v>
       </c>
       <c r="M12" s="5"/>
@@ -5028,13 +5079,13 @@
       <c r="D13" s="31">
         <v>0.89473684210526305</v>
       </c>
-      <c r="E13" s="82">
+      <c r="E13" s="76">
         <v>0.90263157894736801</v>
       </c>
       <c r="F13" s="32">
         <v>0.893421052631579</v>
       </c>
-      <c r="G13" s="82">
+      <c r="G13" s="76">
         <v>0.89605263157894699</v>
       </c>
       <c r="H13" s="32">
@@ -5046,7 +5097,7 @@
       <c r="J13" s="32">
         <v>0.85</v>
       </c>
-      <c r="K13" s="84">
+      <c r="K13" s="77">
         <v>0.89210526315789496</v>
       </c>
       <c r="M13" s="2" t="s">
@@ -5075,13 +5126,13 @@
       <c r="D14" s="25">
         <v>0.88552631578947405</v>
       </c>
-      <c r="E14" s="78">
+      <c r="E14" s="72">
         <v>0.99736842105263201</v>
       </c>
       <c r="F14" s="26">
         <v>0.89144736842105299</v>
       </c>
-      <c r="G14" s="78">
+      <c r="G14" s="72">
         <v>0.99868421052631595</v>
       </c>
       <c r="H14" s="26">
@@ -5093,7 +5144,7 @@
       <c r="J14" s="26">
         <v>0.78486842105263199</v>
       </c>
-      <c r="K14" s="79">
+      <c r="K14" s="73">
         <v>0.95460526315789496</v>
       </c>
       <c r="M14" s="4"/>
@@ -5130,16 +5181,16 @@
       <c r="G15" s="26">
         <v>0.856578947368421</v>
       </c>
-      <c r="H15" s="78">
+      <c r="H15" s="72">
         <v>0.88289473684210495</v>
       </c>
-      <c r="I15" s="78">
+      <c r="I15" s="72">
         <v>0.88026315789473697</v>
       </c>
       <c r="J15" s="26">
         <v>0.84473684210526301</v>
       </c>
-      <c r="K15" s="79">
+      <c r="K15" s="73">
         <v>0.90526315789473699</v>
       </c>
       <c r="M15" s="4"/>
@@ -5167,13 +5218,13 @@
       <c r="D16" s="28">
         <v>0.875</v>
       </c>
-      <c r="E16" s="81">
+      <c r="E16" s="75">
         <v>0.99868421052631595</v>
       </c>
       <c r="F16" s="29">
         <v>0.88355263157894703</v>
       </c>
-      <c r="G16" s="81">
+      <c r="G16" s="75">
         <v>0.99342105263157898</v>
       </c>
       <c r="H16" s="29">
@@ -5185,7 +5236,7 @@
       <c r="J16" s="29">
         <v>0.81118421052631595</v>
       </c>
-      <c r="K16" s="80">
+      <c r="K16" s="74">
         <v>0.96118421052631597</v>
       </c>
       <c r="M16" s="5"/>
@@ -5221,10 +5272,10 @@
       <c r="F17" s="32">
         <v>0.76644736842105299</v>
       </c>
-      <c r="G17" s="82">
+      <c r="G17" s="76">
         <v>0.91447368421052599</v>
       </c>
-      <c r="H17" s="82">
+      <c r="H17" s="76">
         <v>0.84802631578947396</v>
       </c>
       <c r="I17" s="32">
@@ -5233,7 +5284,7 @@
       <c r="J17" s="32">
         <v>0.68552631578947398</v>
       </c>
-      <c r="K17" s="84">
+      <c r="K17" s="77">
         <v>0.91052631578947396</v>
       </c>
       <c r="M17" s="4" t="s">
@@ -5262,7 +5313,7 @@
       <c r="D18" s="25">
         <v>0.66315789473684195</v>
       </c>
-      <c r="E18" s="78">
+      <c r="E18" s="72">
         <v>0.93355263157894697</v>
       </c>
       <c r="F18" s="26">
@@ -5271,7 +5322,7 @@
       <c r="G18" s="26">
         <v>0.92631578947368398</v>
       </c>
-      <c r="H18" s="78">
+      <c r="H18" s="72">
         <v>0.93552631578947398</v>
       </c>
       <c r="I18" s="26">
@@ -5280,7 +5331,7 @@
       <c r="J18" s="26">
         <v>0.61776315789473701</v>
       </c>
-      <c r="K18" s="79">
+      <c r="K18" s="73">
         <v>0.92894736842105297</v>
       </c>
       <c r="M18" s="4"/>
@@ -5314,19 +5365,19 @@
       <c r="F19" s="26">
         <v>0.78421052631579002</v>
       </c>
-      <c r="G19" s="78">
+      <c r="G19" s="72">
         <v>0.879605263157895</v>
       </c>
       <c r="H19" s="26">
         <v>0.84934210526315801</v>
       </c>
-      <c r="I19" s="78">
+      <c r="I19" s="72">
         <v>0.88815789473684204</v>
       </c>
       <c r="J19" s="26">
         <v>0.70263157894736905</v>
       </c>
-      <c r="K19" s="79">
+      <c r="K19" s="73">
         <v>0.86250000000000004</v>
       </c>
       <c r="M19" s="4"/>
@@ -5360,10 +5411,10 @@
       <c r="F20" s="29">
         <v>0.71447368421052604</v>
       </c>
-      <c r="G20" s="81">
+      <c r="G20" s="75">
         <v>0.90131578947368396</v>
       </c>
-      <c r="H20" s="81">
+      <c r="H20" s="75">
         <v>0.932894736842105</v>
       </c>
       <c r="I20" s="29">
@@ -5372,7 +5423,7 @@
       <c r="J20" s="29">
         <v>0.69868421052631602</v>
       </c>
-      <c r="K20" s="80">
+      <c r="K20" s="74">
         <v>0.90789473684210498</v>
       </c>
       <c r="M20" s="5"/>
@@ -5389,7 +5440,7 @@
       <c r="V20" s="29"/>
       <c r="W20" s="30"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
@@ -5399,166 +5450,362 @@
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B22" s="11"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
+    <row r="22" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
+      <c r="A23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="84">
+        <v>0.68421052631579005</v>
+      </c>
+      <c r="E23" s="85">
+        <v>0.83815789473684199</v>
+      </c>
+      <c r="F23" s="85">
+        <v>0.77763157894736901</v>
+      </c>
+      <c r="G23" s="85">
+        <v>0.89013157894736905</v>
+      </c>
+      <c r="H23" s="85">
+        <v>0.87828947368420995</v>
+      </c>
+      <c r="I23" s="85">
+        <v>0.89078947368421102</v>
+      </c>
+      <c r="J23" s="85">
+        <v>0.66710526315789498</v>
+      </c>
+      <c r="K23" s="86">
+        <v>0.89210526315789496</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="87">
+        <v>0.70986842105263204</v>
+      </c>
+      <c r="E24" s="88">
+        <v>0.826315789473684</v>
+      </c>
+      <c r="F24" s="88">
+        <v>0.80197368421052595</v>
+      </c>
+      <c r="G24" s="88">
+        <v>0.84210526315789502</v>
+      </c>
+      <c r="H24" s="88">
+        <v>0.84276315789473699</v>
+      </c>
+      <c r="I24" s="88">
+        <v>0.80657894736842095</v>
+      </c>
+      <c r="J24" s="88">
+        <v>0.69407894736842102</v>
+      </c>
+      <c r="K24" s="89">
+        <v>0.88552631578947405</v>
+      </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="90">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="E25" s="91">
+        <v>0.83157894736842097</v>
+      </c>
+      <c r="F25" s="91">
+        <v>0.83881578947368396</v>
+      </c>
+      <c r="G25" s="91">
+        <v>0.87368421052631595</v>
+      </c>
+      <c r="H25" s="91">
+        <v>0.96644736842105305</v>
+      </c>
+      <c r="I25" s="91">
+        <v>0.92236842105263195</v>
+      </c>
+      <c r="J25" s="91">
+        <v>0.80131578947368398</v>
+      </c>
+      <c r="K25" s="92">
+        <v>0.98355263157894801</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4"/>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="87">
+        <v>0.82039473684210495</v>
+      </c>
+      <c r="E26" s="88">
+        <v>0.85723684210526296</v>
+      </c>
+      <c r="F26" s="88">
+        <v>0.85</v>
+      </c>
+      <c r="G26" s="88">
+        <v>0.83947368421052604</v>
+      </c>
+      <c r="H26" s="88">
+        <v>0.932894736842105</v>
+      </c>
+      <c r="I26" s="88">
+        <v>0.92171052631578898</v>
+      </c>
+      <c r="J26" s="88">
+        <v>0.86315789473684201</v>
+      </c>
+      <c r="K26" s="89">
+        <v>0.90855263157894695</v>
+      </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
+      <c r="A27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="90">
+        <v>0.89473684210526305</v>
+      </c>
+      <c r="E27" s="91">
+        <v>0.99736842105263201</v>
+      </c>
+      <c r="F27" s="91">
+        <v>0.893421052631579</v>
+      </c>
+      <c r="G27" s="91">
+        <v>0.99868421052631595</v>
+      </c>
+      <c r="H27" s="91">
+        <v>0.89802631578947401</v>
+      </c>
+      <c r="I27" s="91">
+        <v>0.90394736842105305</v>
+      </c>
+      <c r="J27" s="91">
+        <v>0.85</v>
+      </c>
+      <c r="K27" s="92">
+        <v>0.95460526315789496</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6">
+        <v>2</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="87">
+        <v>0.87763157894736898</v>
+      </c>
+      <c r="E28" s="88">
+        <v>0.99868421052631595</v>
+      </c>
+      <c r="F28" s="88">
+        <v>0.88355263157894703</v>
+      </c>
+      <c r="G28" s="88">
+        <v>0.99342105263157898</v>
+      </c>
+      <c r="H28" s="88">
+        <v>0.91118421052631604</v>
+      </c>
+      <c r="I28" s="88">
+        <v>0.89473684210526305</v>
+      </c>
+      <c r="J28" s="88">
+        <v>0.84473684210526301</v>
+      </c>
+      <c r="K28" s="89">
+        <v>0.96118421052631597</v>
+      </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
+      <c r="A29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="90">
+        <v>0.70460526315789496</v>
+      </c>
+      <c r="E29" s="91">
+        <v>0.93355263157894697</v>
+      </c>
+      <c r="F29" s="91">
+        <v>0.76644736842105299</v>
+      </c>
+      <c r="G29" s="91">
+        <v>0.92631578947368398</v>
+      </c>
+      <c r="H29" s="91">
+        <v>0.93552631578947398</v>
+      </c>
+      <c r="I29" s="91">
+        <v>0.81842105263157905</v>
+      </c>
+      <c r="J29" s="91">
+        <v>0.68552631578947398</v>
+      </c>
+      <c r="K29" s="92">
+        <v>0.92894736842105297</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6">
+        <v>2</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="87">
+        <v>0.71381578947368396</v>
+      </c>
+      <c r="E30" s="88">
+        <v>0.89407894736842097</v>
+      </c>
+      <c r="F30" s="88">
+        <v>0.78421052631579002</v>
+      </c>
+      <c r="G30" s="88">
+        <v>0.90131578947368396</v>
+      </c>
+      <c r="H30" s="88">
+        <v>0.932894736842105</v>
+      </c>
+      <c r="I30" s="88">
+        <v>0.88815789473684204</v>
+      </c>
+      <c r="J30" s="88">
+        <v>0.70263157894736905</v>
+      </c>
+      <c r="K30" s="89">
+        <v>0.90789473684210498</v>
+      </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
     </row>
     <row r="33" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
     </row>
     <row r="34" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
     </row>
     <row r="35" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
     </row>
     <row r="36" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="12"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
     </row>
     <row r="37" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
     </row>
     <row r="38" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D38" s="10"/>
@@ -5639,86 +5886,6 @@
       <c r="I45" s="10"/>
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
-    </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="10"/>
-      <c r="H46" s="10"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="10"/>
-      <c r="K46" s="10"/>
-    </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="10"/>
-      <c r="K47" s="10"/>
-    </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="10"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10"/>
-      <c r="K48" s="10"/>
-    </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
-      <c r="H49" s="10"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="10"/>
-      <c r="K49" s="10"/>
-    </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
-      <c r="K50" s="10"/>
-    </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="10"/>
-      <c r="H51" s="10"/>
-      <c r="I51" s="10"/>
-      <c r="J51" s="10"/>
-      <c r="K51" s="10"/>
-    </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10"/>
-      <c r="I52" s="10"/>
-      <c r="J52" s="10"/>
-      <c r="K52" s="10"/>
-    </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
-      <c r="H53" s="10"/>
-      <c r="I53" s="10"/>
-      <c r="J53" s="10"/>
-      <c r="K53" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5732,8 +5899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D83308-7EFF-4F48-ACED-83B85BC27520}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5751,19 +5918,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6317,7 +6484,7 @@
         <v>8.0216408588473204E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
@@ -6327,96 +6494,292 @@
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="11"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
+      <c r="A23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="84">
+        <v>3.03868562731382E-2</v>
+      </c>
+      <c r="E23" s="85">
+        <v>0.117286639223007</v>
+      </c>
+      <c r="F23" s="85">
+        <v>6.5847927248548502E-2</v>
+      </c>
+      <c r="G23" s="85">
+        <v>0.10201729872804</v>
+      </c>
+      <c r="H23" s="85">
+        <v>8.6240272378226707E-2</v>
+      </c>
+      <c r="I23" s="85">
+        <v>3.9253773395200801E-2</v>
+      </c>
+      <c r="J23" s="85">
+        <v>6.4101143531386406E-2</v>
+      </c>
+      <c r="K23" s="86">
+        <v>0.12776640253406801</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="87">
+        <v>3.4318598977301697E-2</v>
+      </c>
+      <c r="E24" s="88">
+        <v>0.122736508580892</v>
+      </c>
+      <c r="F24" s="88">
+        <v>3.9771053395802301E-2</v>
+      </c>
+      <c r="G24" s="88">
+        <v>9.4679969933872399E-2</v>
+      </c>
+      <c r="H24" s="88">
+        <v>0.13283211714427101</v>
+      </c>
+      <c r="I24" s="88">
+        <v>0.16052871247372</v>
+      </c>
+      <c r="J24" s="88">
+        <v>4.9256748783368803E-2</v>
+      </c>
+      <c r="K24" s="89">
+        <v>0.131586257106899</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="90">
+        <v>9.2719339740069406E-2</v>
+      </c>
+      <c r="E25" s="91">
+        <v>0.13187831441237799</v>
+      </c>
+      <c r="F25" s="91">
+        <v>7.0874397417510102E-2</v>
+      </c>
+      <c r="G25" s="91">
+        <v>0.12973117788899699</v>
+      </c>
+      <c r="H25" s="91">
+        <v>8.5579717920903201E-2</v>
+      </c>
+      <c r="I25" s="91">
+        <v>2.6822605002492401E-2</v>
+      </c>
+      <c r="J25" s="91">
+        <v>9.4160446031223796E-2</v>
+      </c>
+      <c r="K25" s="92">
+        <v>1.7612257022159E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4"/>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="87">
+        <v>6.37890309848958E-2</v>
+      </c>
+      <c r="E26" s="88">
+        <v>0.14553375772771901</v>
+      </c>
+      <c r="F26" s="88">
+        <v>5.6236212016928397E-2</v>
+      </c>
+      <c r="G26" s="88">
+        <v>0.12541098947832599</v>
+      </c>
+      <c r="H26" s="88">
+        <v>9.4058242108744805E-2</v>
+      </c>
+      <c r="I26" s="88">
+        <v>2.3506889817301101E-2</v>
+      </c>
+      <c r="J26" s="88">
+        <v>7.9421093323091899E-2</v>
+      </c>
+      <c r="K26" s="89">
+        <v>0.110281073646743</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
+      <c r="A27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="90">
+        <v>3.5631747388754201E-2</v>
+      </c>
+      <c r="E27" s="91">
+        <v>8.3217833162325706E-3</v>
+      </c>
+      <c r="F27" s="91">
+        <v>2.25354957520441E-2</v>
+      </c>
+      <c r="G27" s="91">
+        <v>2.7739277720775098E-3</v>
+      </c>
+      <c r="H27" s="91">
+        <v>3.3004203823009698E-2</v>
+      </c>
+      <c r="I27" s="91">
+        <v>3.5658730919610297E-2</v>
+      </c>
+      <c r="J27" s="91">
+        <v>4.0174097886156099E-2</v>
+      </c>
+      <c r="K27" s="92">
+        <v>3.59609005036775E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6">
+        <v>2</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="87">
+        <v>3.44235383690326E-2</v>
+      </c>
+      <c r="E28" s="88">
+        <v>4.1608916581163001E-3</v>
+      </c>
+      <c r="F28" s="88">
+        <v>2.8263111612015199E-2</v>
+      </c>
+      <c r="G28" s="88">
+        <v>1.20114595944115E-2</v>
+      </c>
+      <c r="H28" s="88">
+        <v>2.22022551878471E-2</v>
+      </c>
+      <c r="I28" s="88">
+        <v>3.4674097150969099E-2</v>
+      </c>
+      <c r="J28" s="88">
+        <v>3.7499358771577299E-2</v>
+      </c>
+      <c r="K28" s="89">
+        <v>5.0908376710802901E-2</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
+      <c r="A29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="90">
+        <v>4.9080691532590801E-2</v>
+      </c>
+      <c r="E29" s="91">
+        <v>5.3307970943207703E-2</v>
+      </c>
+      <c r="F29" s="91">
+        <v>3.8141506866066002E-2</v>
+      </c>
+      <c r="G29" s="91">
+        <v>3.4086595136360399E-2</v>
+      </c>
+      <c r="H29" s="91">
+        <v>3.5469415121325801E-2</v>
+      </c>
+      <c r="I29" s="91">
+        <v>0.11745053902239599</v>
+      </c>
+      <c r="J29" s="91">
+        <v>3.5197197627612101E-2</v>
+      </c>
+      <c r="K29" s="92">
+        <v>3.3373705929380403E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6">
+        <v>2</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="87">
+        <v>4.6649226724084697E-2</v>
+      </c>
+      <c r="E30" s="88">
+        <v>7.5360143824942993E-2</v>
+      </c>
+      <c r="F30" s="88">
+        <v>7.72726861247202E-2</v>
+      </c>
+      <c r="G30" s="88">
+        <v>3.54965220531549E-2</v>
+      </c>
+      <c r="H30" s="88">
+        <v>3.1597216937417301E-2</v>
+      </c>
+      <c r="I30" s="88">
+        <v>6.8370426614560997E-2</v>
+      </c>
+      <c r="J30" s="88">
+        <v>3.5333568528285703E-2</v>
+      </c>
+      <c r="K30" s="89">
+        <v>8.0216408588473204E-2</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D31" s="12"/>
@@ -6679,19 +7042,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7449,19 +7812,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8201,7 +8564,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8220,19 +8583,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8971,8 +9334,1064 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40056-F547-48DD-9331-37B657810592}">
   <dimension ref="A1:K53"/>
   <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.21875" customWidth="1"/>
+    <col min="11" max="11" width="5.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="78" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+    </row>
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="55">
+        <v>1</v>
+      </c>
+      <c r="E5" s="56">
+        <v>1</v>
+      </c>
+      <c r="F5" s="56">
+        <v>1</v>
+      </c>
+      <c r="G5" s="56">
+        <v>1</v>
+      </c>
+      <c r="H5" s="56">
+        <v>1</v>
+      </c>
+      <c r="I5" s="56">
+        <v>1</v>
+      </c>
+      <c r="J5" s="56">
+        <v>1</v>
+      </c>
+      <c r="K5" s="57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="49">
+        <v>2</v>
+      </c>
+      <c r="E6" s="50">
+        <v>7</v>
+      </c>
+      <c r="F6" s="50">
+        <v>4</v>
+      </c>
+      <c r="G6" s="50">
+        <v>7</v>
+      </c>
+      <c r="H6" s="50">
+        <v>8</v>
+      </c>
+      <c r="I6" s="50">
+        <v>2</v>
+      </c>
+      <c r="J6" s="50">
+        <v>4</v>
+      </c>
+      <c r="K6" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="49">
+        <v>1</v>
+      </c>
+      <c r="E7" s="50">
+        <v>1</v>
+      </c>
+      <c r="F7" s="50">
+        <v>1</v>
+      </c>
+      <c r="G7" s="50">
+        <v>1</v>
+      </c>
+      <c r="H7" s="50">
+        <v>1</v>
+      </c>
+      <c r="I7" s="50">
+        <v>1</v>
+      </c>
+      <c r="J7" s="50">
+        <v>1</v>
+      </c>
+      <c r="K7" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="52">
+        <v>2</v>
+      </c>
+      <c r="E8" s="53">
+        <v>5</v>
+      </c>
+      <c r="F8" s="53">
+        <v>4</v>
+      </c>
+      <c r="G8" s="53">
+        <v>3</v>
+      </c>
+      <c r="H8" s="53">
+        <v>6</v>
+      </c>
+      <c r="I8" s="53">
+        <v>2</v>
+      </c>
+      <c r="J8" s="53">
+        <v>4</v>
+      </c>
+      <c r="K8" s="54">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="46">
+        <v>1</v>
+      </c>
+      <c r="E9" s="47">
+        <v>1</v>
+      </c>
+      <c r="F9" s="47">
+        <v>1</v>
+      </c>
+      <c r="G9" s="47">
+        <v>1</v>
+      </c>
+      <c r="H9" s="47">
+        <v>1</v>
+      </c>
+      <c r="I9" s="47">
+        <v>1</v>
+      </c>
+      <c r="J9" s="47">
+        <v>1</v>
+      </c>
+      <c r="K9" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="49">
+        <v>4</v>
+      </c>
+      <c r="E10" s="50">
+        <v>8</v>
+      </c>
+      <c r="F10" s="50">
+        <v>2</v>
+      </c>
+      <c r="G10" s="50">
+        <v>9</v>
+      </c>
+      <c r="H10" s="50">
+        <v>10</v>
+      </c>
+      <c r="I10" s="50">
+        <v>2</v>
+      </c>
+      <c r="J10" s="50">
+        <v>2</v>
+      </c>
+      <c r="K10" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="49">
+        <v>1</v>
+      </c>
+      <c r="E11" s="50">
+        <v>1</v>
+      </c>
+      <c r="F11" s="50">
+        <v>1</v>
+      </c>
+      <c r="G11" s="50">
+        <v>1</v>
+      </c>
+      <c r="H11" s="50">
+        <v>1</v>
+      </c>
+      <c r="I11" s="50">
+        <v>1</v>
+      </c>
+      <c r="J11" s="50">
+        <v>1</v>
+      </c>
+      <c r="K11" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="52">
+        <v>2</v>
+      </c>
+      <c r="E12" s="53">
+        <v>5</v>
+      </c>
+      <c r="F12" s="53">
+        <v>2</v>
+      </c>
+      <c r="G12" s="53">
+        <v>10</v>
+      </c>
+      <c r="H12" s="53">
+        <v>10</v>
+      </c>
+      <c r="I12" s="53">
+        <v>2</v>
+      </c>
+      <c r="J12" s="53">
+        <v>4</v>
+      </c>
+      <c r="K12" s="54">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="46">
+        <v>1</v>
+      </c>
+      <c r="E13" s="47">
+        <v>1</v>
+      </c>
+      <c r="F13" s="47">
+        <v>1</v>
+      </c>
+      <c r="G13" s="47">
+        <v>1</v>
+      </c>
+      <c r="H13" s="47">
+        <v>1</v>
+      </c>
+      <c r="I13" s="47">
+        <v>1</v>
+      </c>
+      <c r="J13" s="47">
+        <v>1</v>
+      </c>
+      <c r="K13" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="49">
+        <v>2</v>
+      </c>
+      <c r="E14" s="50">
+        <v>7</v>
+      </c>
+      <c r="F14" s="50">
+        <v>2</v>
+      </c>
+      <c r="G14" s="50">
+        <v>3</v>
+      </c>
+      <c r="H14" s="50">
+        <v>7</v>
+      </c>
+      <c r="I14" s="50">
+        <v>3</v>
+      </c>
+      <c r="J14" s="50">
+        <v>2</v>
+      </c>
+      <c r="K14" s="51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="49">
+        <v>1</v>
+      </c>
+      <c r="E15" s="50">
+        <v>1</v>
+      </c>
+      <c r="F15" s="50">
+        <v>1</v>
+      </c>
+      <c r="G15" s="50">
+        <v>1</v>
+      </c>
+      <c r="H15" s="50">
+        <v>1</v>
+      </c>
+      <c r="I15" s="50">
+        <v>1</v>
+      </c>
+      <c r="J15" s="50">
+        <v>1</v>
+      </c>
+      <c r="K15" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="52">
+        <v>2</v>
+      </c>
+      <c r="E16" s="53">
+        <v>3</v>
+      </c>
+      <c r="F16" s="53">
+        <v>2</v>
+      </c>
+      <c r="G16" s="53">
+        <v>5</v>
+      </c>
+      <c r="H16" s="53">
+        <v>8</v>
+      </c>
+      <c r="I16" s="53">
+        <v>7</v>
+      </c>
+      <c r="J16" s="53">
+        <v>4</v>
+      </c>
+      <c r="K16" s="54">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="46">
+        <v>1</v>
+      </c>
+      <c r="E17" s="47">
+        <v>1</v>
+      </c>
+      <c r="F17" s="47">
+        <v>1</v>
+      </c>
+      <c r="G17" s="47">
+        <v>1</v>
+      </c>
+      <c r="H17" s="47">
+        <v>1</v>
+      </c>
+      <c r="I17" s="47">
+        <v>1</v>
+      </c>
+      <c r="J17" s="47">
+        <v>1</v>
+      </c>
+      <c r="K17" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="C18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="49">
+        <v>2</v>
+      </c>
+      <c r="E18" s="50">
+        <v>10</v>
+      </c>
+      <c r="F18" s="50">
+        <v>2</v>
+      </c>
+      <c r="G18" s="50">
+        <v>3</v>
+      </c>
+      <c r="H18" s="50">
+        <v>7</v>
+      </c>
+      <c r="I18" s="50">
+        <v>2</v>
+      </c>
+      <c r="J18" s="50">
+        <v>2</v>
+      </c>
+      <c r="K18" s="51">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="49">
+        <v>1</v>
+      </c>
+      <c r="E19" s="50">
+        <v>1</v>
+      </c>
+      <c r="F19" s="50">
+        <v>1</v>
+      </c>
+      <c r="G19" s="50">
+        <v>1</v>
+      </c>
+      <c r="H19" s="50">
+        <v>1</v>
+      </c>
+      <c r="I19" s="50">
+        <v>1</v>
+      </c>
+      <c r="J19" s="50">
+        <v>1</v>
+      </c>
+      <c r="K19" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="52">
+        <v>5</v>
+      </c>
+      <c r="E20" s="53">
+        <v>9</v>
+      </c>
+      <c r="F20" s="53">
+        <v>3</v>
+      </c>
+      <c r="G20" s="53">
+        <v>9</v>
+      </c>
+      <c r="H20" s="53">
+        <v>7</v>
+      </c>
+      <c r="I20" s="53">
+        <v>4</v>
+      </c>
+      <c r="J20" s="53">
+        <v>2</v>
+      </c>
+      <c r="K20" s="54">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="93">
+        <v>1</v>
+      </c>
+      <c r="E23" s="94">
+        <v>7</v>
+      </c>
+      <c r="F23" s="94">
+        <v>1</v>
+      </c>
+      <c r="G23" s="94">
+        <v>7</v>
+      </c>
+      <c r="H23" s="94">
+        <v>8</v>
+      </c>
+      <c r="I23" s="94">
+        <v>1</v>
+      </c>
+      <c r="J23" s="94">
+        <v>1</v>
+      </c>
+      <c r="K23" s="95">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="96">
+        <v>1</v>
+      </c>
+      <c r="E24" s="97">
+        <v>5</v>
+      </c>
+      <c r="F24" s="97">
+        <v>1</v>
+      </c>
+      <c r="G24" s="97">
+        <v>3</v>
+      </c>
+      <c r="H24" s="97">
+        <v>6</v>
+      </c>
+      <c r="I24" s="97">
+        <v>1</v>
+      </c>
+      <c r="J24" s="97">
+        <v>1</v>
+      </c>
+      <c r="K24" s="98">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="99">
+        <v>1</v>
+      </c>
+      <c r="E25" s="100">
+        <v>8</v>
+      </c>
+      <c r="F25" s="100">
+        <v>1</v>
+      </c>
+      <c r="G25" s="100">
+        <v>9</v>
+      </c>
+      <c r="H25" s="100">
+        <v>10</v>
+      </c>
+      <c r="I25" s="100">
+        <v>2</v>
+      </c>
+      <c r="J25" s="100">
+        <v>1</v>
+      </c>
+      <c r="K25" s="101">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4"/>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="96">
+        <v>2</v>
+      </c>
+      <c r="E26" s="97">
+        <v>5</v>
+      </c>
+      <c r="F26" s="97">
+        <v>1</v>
+      </c>
+      <c r="G26" s="97">
+        <v>10</v>
+      </c>
+      <c r="H26" s="97">
+        <v>10</v>
+      </c>
+      <c r="I26" s="97">
+        <v>2</v>
+      </c>
+      <c r="J26" s="97">
+        <v>1</v>
+      </c>
+      <c r="K26" s="98">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="99">
+        <v>1</v>
+      </c>
+      <c r="E27" s="100">
+        <v>7</v>
+      </c>
+      <c r="F27" s="100">
+        <v>1</v>
+      </c>
+      <c r="G27" s="100">
+        <v>3</v>
+      </c>
+      <c r="H27" s="100">
+        <v>7</v>
+      </c>
+      <c r="I27" s="100">
+        <v>3</v>
+      </c>
+      <c r="J27" s="100">
+        <v>1</v>
+      </c>
+      <c r="K27" s="101">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6">
+        <v>2</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="96">
+        <v>1</v>
+      </c>
+      <c r="E28" s="97">
+        <v>3</v>
+      </c>
+      <c r="F28" s="97">
+        <v>2</v>
+      </c>
+      <c r="G28" s="97">
+        <v>5</v>
+      </c>
+      <c r="H28" s="97">
+        <v>8</v>
+      </c>
+      <c r="I28" s="97">
+        <v>7</v>
+      </c>
+      <c r="J28" s="97">
+        <v>1</v>
+      </c>
+      <c r="K28" s="98">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="99">
+        <v>1</v>
+      </c>
+      <c r="E29" s="100">
+        <v>10</v>
+      </c>
+      <c r="F29" s="100">
+        <v>1</v>
+      </c>
+      <c r="G29" s="100">
+        <v>3</v>
+      </c>
+      <c r="H29" s="100">
+        <v>7</v>
+      </c>
+      <c r="I29" s="100">
+        <v>2</v>
+      </c>
+      <c r="J29" s="100">
+        <v>1</v>
+      </c>
+      <c r="K29" s="101">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6">
+        <v>2</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="96">
+        <v>5</v>
+      </c>
+      <c r="E30" s="97">
+        <v>9</v>
+      </c>
+      <c r="F30" s="97">
+        <v>1</v>
+      </c>
+      <c r="G30" s="97">
+        <v>9</v>
+      </c>
+      <c r="H30" s="97">
+        <v>7</v>
+      </c>
+      <c r="I30" s="97">
+        <v>1</v>
+      </c>
+      <c r="J30" s="97">
+        <v>1</v>
+      </c>
+      <c r="K30" s="98">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+    </row>
+    <row r="39" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+    </row>
+    <row r="40" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+    </row>
+    <row r="41" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+    </row>
+    <row r="42" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+    </row>
+    <row r="43" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+    </row>
+    <row r="44" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+    </row>
+    <row r="45" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+    </row>
+    <row r="46" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
+    </row>
+    <row r="47" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="10"/>
+    </row>
+    <row r="48" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="10"/>
+    </row>
+    <row r="49" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
+    </row>
+    <row r="50" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+      <c r="K50" s="10"/>
+    </row>
+    <row r="51" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="10"/>
+      <c r="K51" s="10"/>
+    </row>
+    <row r="52" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10"/>
+      <c r="K52" s="10"/>
+    </row>
+    <row r="53" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10"/>
+      <c r="K53" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5843C1-20CB-4050-94D7-D7DDEA36873C}">
+  <dimension ref="A1:K53"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8990,789 +10409,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-    </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="55">
-        <v>1</v>
-      </c>
-      <c r="E5" s="56">
-        <v>1</v>
-      </c>
-      <c r="F5" s="56">
-        <v>1</v>
-      </c>
-      <c r="G5" s="56">
-        <v>1</v>
-      </c>
-      <c r="H5" s="56">
-        <v>1</v>
-      </c>
-      <c r="I5" s="56">
-        <v>1</v>
-      </c>
-      <c r="J5" s="56">
-        <v>1</v>
-      </c>
-      <c r="K5" s="57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="49">
-        <v>2</v>
-      </c>
-      <c r="E6" s="50">
-        <v>7</v>
-      </c>
-      <c r="F6" s="50">
-        <v>4</v>
-      </c>
-      <c r="G6" s="50">
-        <v>7</v>
-      </c>
-      <c r="H6" s="50">
-        <v>8</v>
-      </c>
-      <c r="I6" s="50">
-        <v>2</v>
-      </c>
-      <c r="J6" s="50">
-        <v>4</v>
-      </c>
-      <c r="K6" s="51">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="1">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="49">
-        <v>1</v>
-      </c>
-      <c r="E7" s="50">
-        <v>1</v>
-      </c>
-      <c r="F7" s="50">
-        <v>1</v>
-      </c>
-      <c r="G7" s="50">
-        <v>1</v>
-      </c>
-      <c r="H7" s="50">
-        <v>1</v>
-      </c>
-      <c r="I7" s="50">
-        <v>1</v>
-      </c>
-      <c r="J7" s="50">
-        <v>1</v>
-      </c>
-      <c r="K7" s="51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="52">
-        <v>2</v>
-      </c>
-      <c r="E8" s="53">
-        <v>5</v>
-      </c>
-      <c r="F8" s="53">
-        <v>4</v>
-      </c>
-      <c r="G8" s="53">
-        <v>3</v>
-      </c>
-      <c r="H8" s="53">
-        <v>6</v>
-      </c>
-      <c r="I8" s="53">
-        <v>2</v>
-      </c>
-      <c r="J8" s="53">
-        <v>4</v>
-      </c>
-      <c r="K8" s="54">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="3">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="D9" s="46">
-        <v>1</v>
-      </c>
-      <c r="E9" s="47">
-        <v>1</v>
-      </c>
-      <c r="F9" s="47">
-        <v>1</v>
-      </c>
-      <c r="G9" s="47">
-        <v>1</v>
-      </c>
-      <c r="H9" s="47">
-        <v>1</v>
-      </c>
-      <c r="I9" s="47">
-        <v>1</v>
-      </c>
-      <c r="J9" s="47">
-        <v>1</v>
-      </c>
-      <c r="K9" s="48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="C10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="49">
-        <v>4</v>
-      </c>
-      <c r="E10" s="50">
-        <v>8</v>
-      </c>
-      <c r="F10" s="50">
-        <v>2</v>
-      </c>
-      <c r="G10" s="50">
-        <v>9</v>
-      </c>
-      <c r="H10" s="50">
-        <v>10</v>
-      </c>
-      <c r="I10" s="50">
-        <v>2</v>
-      </c>
-      <c r="J10" s="50">
-        <v>2</v>
-      </c>
-      <c r="K10" s="51">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="1">
-        <v>2</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="49">
-        <v>1</v>
-      </c>
-      <c r="E11" s="50">
-        <v>1</v>
-      </c>
-      <c r="F11" s="50">
-        <v>1</v>
-      </c>
-      <c r="G11" s="50">
-        <v>1</v>
-      </c>
-      <c r="H11" s="50">
-        <v>1</v>
-      </c>
-      <c r="I11" s="50">
-        <v>1</v>
-      </c>
-      <c r="J11" s="50">
-        <v>1</v>
-      </c>
-      <c r="K11" s="51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="52">
-        <v>2</v>
-      </c>
-      <c r="E12" s="53">
-        <v>5</v>
-      </c>
-      <c r="F12" s="53">
-        <v>2</v>
-      </c>
-      <c r="G12" s="53">
-        <v>10</v>
-      </c>
-      <c r="H12" s="53">
-        <v>10</v>
-      </c>
-      <c r="I12" s="53">
-        <v>2</v>
-      </c>
-      <c r="J12" s="53">
-        <v>4</v>
-      </c>
-      <c r="K12" s="54">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="3">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3">
-        <v>1</v>
-      </c>
-      <c r="D13" s="46">
-        <v>1</v>
-      </c>
-      <c r="E13" s="47">
-        <v>1</v>
-      </c>
-      <c r="F13" s="47">
-        <v>1</v>
-      </c>
-      <c r="G13" s="47">
-        <v>1</v>
-      </c>
-      <c r="H13" s="47">
-        <v>1</v>
-      </c>
-      <c r="I13" s="47">
-        <v>1</v>
-      </c>
-      <c r="J13" s="47">
-        <v>1</v>
-      </c>
-      <c r="K13" s="48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="C14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="49">
-        <v>2</v>
-      </c>
-      <c r="E14" s="50">
-        <v>7</v>
-      </c>
-      <c r="F14" s="50">
-        <v>2</v>
-      </c>
-      <c r="G14" s="50">
-        <v>3</v>
-      </c>
-      <c r="H14" s="50">
-        <v>7</v>
-      </c>
-      <c r="I14" s="50">
-        <v>3</v>
-      </c>
-      <c r="J14" s="50">
-        <v>2</v>
-      </c>
-      <c r="K14" s="51">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="1">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="49">
-        <v>1</v>
-      </c>
-      <c r="E15" s="50">
-        <v>1</v>
-      </c>
-      <c r="F15" s="50">
-        <v>1</v>
-      </c>
-      <c r="G15" s="50">
-        <v>1</v>
-      </c>
-      <c r="H15" s="50">
-        <v>1</v>
-      </c>
-      <c r="I15" s="50">
-        <v>1</v>
-      </c>
-      <c r="J15" s="50">
-        <v>1</v>
-      </c>
-      <c r="K15" s="51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="52">
-        <v>2</v>
-      </c>
-      <c r="E16" s="53">
-        <v>3</v>
-      </c>
-      <c r="F16" s="53">
-        <v>2</v>
-      </c>
-      <c r="G16" s="53">
-        <v>5</v>
-      </c>
-      <c r="H16" s="53">
-        <v>8</v>
-      </c>
-      <c r="I16" s="53">
-        <v>7</v>
-      </c>
-      <c r="J16" s="53">
-        <v>4</v>
-      </c>
-      <c r="K16" s="54">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" s="46">
-        <v>1</v>
-      </c>
-      <c r="E17" s="47">
-        <v>1</v>
-      </c>
-      <c r="F17" s="47">
-        <v>1</v>
-      </c>
-      <c r="G17" s="47">
-        <v>1</v>
-      </c>
-      <c r="H17" s="47">
-        <v>1</v>
-      </c>
-      <c r="I17" s="47">
-        <v>1</v>
-      </c>
-      <c r="J17" s="47">
-        <v>1</v>
-      </c>
-      <c r="K17" s="48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="C18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="49">
-        <v>2</v>
-      </c>
-      <c r="E18" s="50">
-        <v>10</v>
-      </c>
-      <c r="F18" s="50">
-        <v>2</v>
-      </c>
-      <c r="G18" s="50">
-        <v>3</v>
-      </c>
-      <c r="H18" s="50">
-        <v>7</v>
-      </c>
-      <c r="I18" s="50">
-        <v>2</v>
-      </c>
-      <c r="J18" s="50">
-        <v>2</v>
-      </c>
-      <c r="K18" s="51">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="1">
-        <v>2</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="49">
-        <v>1</v>
-      </c>
-      <c r="E19" s="50">
-        <v>1</v>
-      </c>
-      <c r="F19" s="50">
-        <v>1</v>
-      </c>
-      <c r="G19" s="50">
-        <v>1</v>
-      </c>
-      <c r="H19" s="50">
-        <v>1</v>
-      </c>
-      <c r="I19" s="50">
-        <v>1</v>
-      </c>
-      <c r="J19" s="50">
-        <v>1</v>
-      </c>
-      <c r="K19" s="51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="52">
-        <v>5</v>
-      </c>
-      <c r="E20" s="53">
-        <v>9</v>
-      </c>
-      <c r="F20" s="53">
-        <v>3</v>
-      </c>
-      <c r="G20" s="53">
-        <v>9</v>
-      </c>
-      <c r="H20" s="53">
-        <v>7</v>
-      </c>
-      <c r="I20" s="53">
-        <v>4</v>
-      </c>
-      <c r="J20" s="53">
-        <v>2</v>
-      </c>
-      <c r="K20" s="54">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="11"/>
-    </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-    </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-    </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-    </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
-      <c r="K40" s="10"/>
-    </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="10"/>
-    </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
-      <c r="K42" s="10"/>
-    </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="10"/>
-      <c r="K43" s="10"/>
-    </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="10"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="10"/>
-      <c r="K44" s="10"/>
-    </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
-      <c r="H45" s="10"/>
-      <c r="I45" s="10"/>
-      <c r="J45" s="10"/>
-      <c r="K45" s="10"/>
-    </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="10"/>
-      <c r="H46" s="10"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="10"/>
-      <c r="K46" s="10"/>
-    </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="10"/>
-      <c r="K47" s="10"/>
-    </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="10"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10"/>
-      <c r="K48" s="10"/>
-    </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
-      <c r="H49" s="10"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="10"/>
-      <c r="K49" s="10"/>
-    </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
-      <c r="K50" s="10"/>
-    </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="10"/>
-      <c r="H51" s="10"/>
-      <c r="I51" s="10"/>
-      <c r="J51" s="10"/>
-      <c r="K51" s="10"/>
-    </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10"/>
-      <c r="I52" s="10"/>
-      <c r="J52" s="10"/>
-      <c r="K52" s="10"/>
-    </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
-      <c r="H53" s="10"/>
-      <c r="I53" s="10"/>
-      <c r="J53" s="10"/>
-      <c r="K53" s="10"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5843C1-20CB-4050-94D7-D7DDEA36873C}">
-  <dimension ref="A1:K53"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10535,24 +11184,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
     </row>
     <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10562,29 +11211,29 @@
       <c r="E3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="71" t="s">
+      <c r="F3" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
       <c r="I3" s="14" t="s">
         <v>15</v>
       </c>
       <c r="J3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="72" t="s">
+      <c r="K3" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="73"/>
-      <c r="M3" s="72" t="s">
+      <c r="L3" s="81"/>
+      <c r="M3" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="73"/>
-      <c r="O3" s="72" t="s">
+      <c r="N3" s="81"/>
+      <c r="O3" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="74"/>
+      <c r="P3" s="82"/>
     </row>
     <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">

</xml_diff>

<commit_message>
highlighted motorfailure best results
</commit_message>
<xml_diff>
--- a/results_analysis/spark_motorFailure_02_hold_01.xlsx
+++ b/results_analysis/spark_motorFailure_02_hold_01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAC7202-C732-46D8-9F3D-1430D13083CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D7C98E-E908-499B-8A1E-7144E78DA068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="734" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="734" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_best" sheetId="11" r:id="rId1"/>
@@ -1081,21 +1081,21 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="78" t="s">
         <v>14</v>
       </c>
@@ -1110,8 +1110,8 @@
       <c r="J1" s="78"/>
       <c r="K1" s="78"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>0.94736842105263197</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -1211,7 +1211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1">
         <v>2</v>
@@ -1244,7 +1244,7 @@
         <v>0.92763157894736903</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
@@ -1275,7 +1275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>0.85526315789473695</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -1340,7 +1340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1">
         <v>2</v>
@@ -1373,7 +1373,7 @@
         <v>0.89473684210526305</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
@@ -1404,7 +1404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>0.94078947368421095</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -1469,7 +1469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1">
         <v>2</v>
@@ -1502,7 +1502,7 @@
         <v>0.93421052631579005</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
@@ -1533,7 +1533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>0.96710526315789502</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -1598,7 +1598,7 @@
         <v>0.97368421052631604</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -1631,7 +1631,7 @@
         <v>0.96710526315789502</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
@@ -1662,7 +1662,7 @@
         <v>0.98684210526315796</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
@@ -1672,7 +1672,7 @@
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
@@ -1683,7 +1683,7 @@
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
@@ -1693,7 +1693,7 @@
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
@@ -1703,7 +1703,7 @@
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
@@ -1713,7 +1713,7 @@
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
@@ -1723,7 +1723,7 @@
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
@@ -1733,7 +1733,7 @@
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
@@ -1743,7 +1743,7 @@
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
@@ -1753,7 +1753,7 @@
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
@@ -1763,7 +1763,7 @@
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
@@ -1773,7 +1773,7 @@
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
@@ -1783,7 +1783,7 @@
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
     </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
@@ -1793,7 +1793,7 @@
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
     </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
@@ -1803,7 +1803,7 @@
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
     </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
@@ -1813,7 +1813,7 @@
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
     </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
@@ -1823,7 +1823,7 @@
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
     </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -1833,7 +1833,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -1843,7 +1843,7 @@
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -1853,7 +1853,7 @@
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -1863,7 +1863,7 @@
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -1873,7 +1873,7 @@
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -1883,7 +1883,7 @@
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -1893,7 +1893,7 @@
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -1903,7 +1903,7 @@
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -1913,7 +1913,7 @@
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -1923,7 +1923,7 @@
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
     </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
@@ -1933,7 +1933,7 @@
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
     </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -1943,7 +1943,7 @@
       <c r="J48" s="10"/>
       <c r="K48" s="10"/>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
@@ -1953,7 +1953,7 @@
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
@@ -1963,7 +1963,7 @@
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
@@ -1973,7 +1973,7 @@
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
@@ -1983,7 +1983,7 @@
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
@@ -2010,25 +2010,25 @@
       <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="78" t="s">
         <v>21</v>
       </c>
@@ -2050,8 +2050,8 @@
       <c r="Q1" s="78"/>
       <c r="R1" s="78"/>
     </row>
-    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="83" t="s">
         <v>6</v>
       </c>
@@ -2085,7 +2085,7 @@
       </c>
       <c r="S3" s="82"/>
     </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>1024.001</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -2257,7 +2257,7 @@
         <v>1024.001</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1">
         <v>2</v>
@@ -2314,7 +2314,7 @@
         <v>1024.001</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
@@ -2369,7 +2369,7 @@
         <v>1024.001</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -2482,7 +2482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1">
         <v>2</v>
@@ -2539,7 +2539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
@@ -2594,7 +2594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>4.8828125E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -2707,7 +2707,7 @@
         <v>16.0009765625</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1">
         <v>2</v>
@@ -2764,7 +2764,7 @@
         <v>1.66015625E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
@@ -2819,7 +2819,7 @@
         <v>128.0009765625</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>16.0009765625</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -2932,7 +2932,7 @@
         <v>128.0009765625</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -2989,7 +2989,7 @@
         <v>128.0009765625</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
@@ -3044,10 +3044,10 @@
         <v>256.0009765625</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
     </row>
-    <row r="37" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -3064,7 +3064,7 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -3081,7 +3081,7 @@
       <c r="Q38" s="10"/>
       <c r="R38" s="10"/>
     </row>
-    <row r="39" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -3098,7 +3098,7 @@
       <c r="Q39" s="10"/>
       <c r="R39" s="10"/>
     </row>
-    <row r="40" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -3115,7 +3115,7 @@
       <c r="Q40" s="10"/>
       <c r="R40" s="10"/>
     </row>
-    <row r="41" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -3132,7 +3132,7 @@
       <c r="Q41" s="10"/>
       <c r="R41" s="10"/>
     </row>
-    <row r="42" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -3149,7 +3149,7 @@
       <c r="Q42" s="10"/>
       <c r="R42" s="10"/>
     </row>
-    <row r="43" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -3166,7 +3166,7 @@
       <c r="Q43" s="10"/>
       <c r="R43" s="10"/>
     </row>
-    <row r="44" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -3183,7 +3183,7 @@
       <c r="Q44" s="10"/>
       <c r="R44" s="10"/>
     </row>
-    <row r="45" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -3200,7 +3200,7 @@
       <c r="Q45" s="10"/>
       <c r="R45" s="10"/>
     </row>
-    <row r="46" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -3217,7 +3217,7 @@
       <c r="Q46" s="10"/>
       <c r="R46" s="10"/>
     </row>
-    <row r="47" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
@@ -3234,7 +3234,7 @@
       <c r="Q47" s="10"/>
       <c r="R47" s="10"/>
     </row>
-    <row r="48" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -3251,7 +3251,7 @@
       <c r="Q48" s="10"/>
       <c r="R48" s="10"/>
     </row>
-    <row r="49" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
@@ -3268,7 +3268,7 @@
       <c r="Q49" s="10"/>
       <c r="R49" s="10"/>
     </row>
-    <row r="50" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
@@ -3285,7 +3285,7 @@
       <c r="Q50" s="10"/>
       <c r="R50" s="10"/>
     </row>
-    <row r="51" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
@@ -3302,7 +3302,7 @@
       <c r="Q51" s="10"/>
       <c r="R51" s="10"/>
     </row>
-    <row r="52" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
@@ -3319,7 +3319,7 @@
       <c r="Q52" s="10"/>
       <c r="R52" s="10"/>
     </row>
-    <row r="53" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
@@ -3360,17 +3360,17 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -3378,7 +3378,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -3482,7 +3482,7 @@
       <c r="V4" s="23"/>
       <c r="W4" s="24"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
@@ -3510,7 +3510,7 @@
       <c r="V5" s="25"/>
       <c r="W5" s="25"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1">
         <v>2</v>
@@ -3542,7 +3542,7 @@
       <c r="V6" s="26"/>
       <c r="W6" s="27"/>
     </row>
-    <row r="7" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
@@ -3570,7 +3570,7 @@
       <c r="V7" s="29"/>
       <c r="W7" s="30"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -3606,7 +3606,7 @@
       <c r="V8" s="32"/>
       <c r="W8" s="33"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
@@ -3634,7 +3634,7 @@
       <c r="V9" s="26"/>
       <c r="W9" s="27"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1">
         <v>2</v>
@@ -3666,7 +3666,7 @@
       <c r="V10" s="26"/>
       <c r="W10" s="27"/>
     </row>
-    <row r="11" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6" t="s">
@@ -3694,7 +3694,7 @@
       <c r="V11" s="29"/>
       <c r="W11" s="30"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -3730,7 +3730,7 @@
       <c r="V12" s="32"/>
       <c r="W12" s="33"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
@@ -3758,7 +3758,7 @@
       <c r="V13" s="26"/>
       <c r="W13" s="27"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1">
         <v>2</v>
@@ -3790,7 +3790,7 @@
       <c r="V14" s="26"/>
       <c r="W14" s="27"/>
     </row>
-    <row r="15" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6" t="s">
@@ -3818,7 +3818,7 @@
       <c r="V15" s="29"/>
       <c r="W15" s="30"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
@@ -3854,7 +3854,7 @@
       <c r="V16" s="32"/>
       <c r="W16" s="33"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
@@ -3882,7 +3882,7 @@
       <c r="V17" s="26"/>
       <c r="W17" s="27"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1">
         <v>2</v>
@@ -3914,7 +3914,7 @@
       <c r="V18" s="26"/>
       <c r="W18" s="27"/>
     </row>
-    <row r="19" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6" t="s">
@@ -3942,7 +3942,7 @@
       <c r="V19" s="29"/>
       <c r="W19" s="30"/>
     </row>
-    <row r="21" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
@@ -4054,7 +4054,7 @@
       <c r="V23" s="23"/>
       <c r="W23" s="24"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
@@ -4082,7 +4082,7 @@
       <c r="V24" s="26"/>
       <c r="W24" s="27"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1">
         <v>2</v>
@@ -4114,7 +4114,7 @@
       <c r="V25" s="26"/>
       <c r="W25" s="27"/>
     </row>
-    <row r="26" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6" t="s">
@@ -4142,7 +4142,7 @@
       <c r="V26" s="29"/>
       <c r="W26" s="30"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>3</v>
       </c>
@@ -4178,7 +4178,7 @@
       <c r="V27" s="32"/>
       <c r="W27" s="33"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
@@ -4206,7 +4206,7 @@
       <c r="V28" s="26"/>
       <c r="W28" s="27"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1">
         <v>2</v>
@@ -4238,7 +4238,7 @@
       <c r="V29" s="26"/>
       <c r="W29" s="27"/>
     </row>
-    <row r="30" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6" t="s">
@@ -4266,7 +4266,7 @@
       <c r="V30" s="29"/>
       <c r="W30" s="30"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>4</v>
       </c>
@@ -4302,7 +4302,7 @@
       <c r="V31" s="32"/>
       <c r="W31" s="33"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
@@ -4330,7 +4330,7 @@
       <c r="V32" s="26"/>
       <c r="W32" s="27"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="1">
         <v>2</v>
@@ -4362,7 +4362,7 @@
       <c r="V33" s="26"/>
       <c r="W33" s="27"/>
     </row>
-    <row r="34" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6" t="s">
@@ -4390,7 +4390,7 @@
       <c r="V34" s="29"/>
       <c r="W34" s="30"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>5</v>
       </c>
@@ -4426,7 +4426,7 @@
       <c r="V35" s="32"/>
       <c r="W35" s="33"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
@@ -4454,7 +4454,7 @@
       <c r="V36" s="26"/>
       <c r="W36" s="27"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="1">
         <v>2</v>
@@ -4486,7 +4486,7 @@
       <c r="V37" s="26"/>
       <c r="W37" s="27"/>
     </row>
-    <row r="38" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6" t="s">
@@ -4528,29 +4528,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2.33203125" customWidth="1"/>
+    <col min="12" max="12" width="2.28515625" customWidth="1"/>
     <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="78" t="s">
         <v>14</v>
       </c>
@@ -4565,12 +4565,12 @@
       <c r="J1" s="78"/>
       <c r="K1" s="78"/>
     </row>
-    <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -4638,7 +4638,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -4690,7 +4690,7 @@
       <c r="V5" s="23"/>
       <c r="W5" s="24"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -4733,7 +4733,7 @@
       <c r="V6" s="26"/>
       <c r="W6" s="27"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1">
         <v>2</v>
@@ -4781,7 +4781,7 @@
       <c r="V7" s="26"/>
       <c r="W7" s="27"/>
     </row>
-    <row r="8" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
@@ -4825,7 +4825,7 @@
       <c r="V8" s="29"/>
       <c r="W8" s="30"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -4877,7 +4877,7 @@
       <c r="V9" s="32"/>
       <c r="W9" s="33"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -4920,7 +4920,7 @@
       <c r="V10" s="26"/>
       <c r="W10" s="27"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1">
         <v>2</v>
@@ -4968,7 +4968,7 @@
       <c r="V11" s="26"/>
       <c r="W11" s="27"/>
     </row>
-    <row r="12" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
@@ -5012,7 +5012,7 @@
       <c r="V12" s="29"/>
       <c r="W12" s="30"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -5064,7 +5064,7 @@
       <c r="V13" s="32"/>
       <c r="W13" s="33"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -5107,7 +5107,7 @@
       <c r="V14" s="26"/>
       <c r="W14" s="27"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1">
         <v>2</v>
@@ -5155,7 +5155,7 @@
       <c r="V15" s="26"/>
       <c r="W15" s="27"/>
     </row>
-    <row r="16" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
@@ -5199,7 +5199,7 @@
       <c r="V16" s="29"/>
       <c r="W16" s="30"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -5251,7 +5251,7 @@
       <c r="V17" s="32"/>
       <c r="W17" s="33"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -5294,7 +5294,7 @@
       <c r="V18" s="26"/>
       <c r="W18" s="27"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -5342,7 +5342,7 @@
       <c r="V19" s="26"/>
       <c r="W19" s="27"/>
     </row>
-    <row r="20" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
@@ -5386,7 +5386,7 @@
       <c r="V20" s="29"/>
       <c r="W20" s="30"/>
     </row>
-    <row r="21" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
@@ -5396,7 +5396,7 @@
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
     </row>
-    <row r="22" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
@@ -5462,7 +5462,7 @@
         <v>0.89210526315789496</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="1">
         <v>2</v>
@@ -5492,7 +5492,7 @@
         <v>0.88552631578947405</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>3</v>
       </c>
@@ -5525,7 +5525,7 @@
         <v>0.98355263157894801</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="1">
         <v>2</v>
@@ -5555,7 +5555,7 @@
         <v>0.90855263157894695</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>4</v>
       </c>
@@ -5588,7 +5588,7 @@
         <v>0.95460526315789496</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="6">
         <v>2</v>
@@ -5619,7 +5619,7 @@
         <v>0.96118421052631597</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>5</v>
       </c>
@@ -5652,7 +5652,7 @@
         <v>0.92894736842105297</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="6">
         <v>2</v>
@@ -5683,7 +5683,7 @@
         <v>0.90789473684210498</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
@@ -5693,7 +5693,7 @@
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
@@ -5703,7 +5703,7 @@
       <c r="J32" s="10"/>
       <c r="K32" s="10"/>
     </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
@@ -5713,7 +5713,7 @@
       <c r="J33" s="10"/>
       <c r="K33" s="10"/>
     </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
@@ -5723,7 +5723,7 @@
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
     </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
@@ -5733,7 +5733,7 @@
       <c r="J35" s="10"/>
       <c r="K35" s="10"/>
     </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
@@ -5743,7 +5743,7 @@
       <c r="J36" s="10"/>
       <c r="K36" s="10"/>
     </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
@@ -5753,7 +5753,7 @@
       <c r="J37" s="10"/>
       <c r="K37" s="10"/>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -5763,7 +5763,7 @@
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -5773,7 +5773,7 @@
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -5783,7 +5783,7 @@
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -5793,7 +5793,7 @@
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -5803,7 +5803,7 @@
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -5813,7 +5813,7 @@
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -5823,7 +5823,7 @@
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -5849,21 +5849,21 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="78" t="s">
         <v>14</v>
       </c>
@@ -5878,8 +5878,8 @@
       <c r="J1" s="78"/>
       <c r="K1" s="78"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>34</v>
       </c>
@@ -5914,7 +5914,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -5949,7 +5949,7 @@
         <v>9.8327816487651695E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -5979,7 +5979,7 @@
         <v>0.12776640253406801</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1">
         <v>2</v>
@@ -6012,7 +6012,7 @@
         <v>7.7250900321565605E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
@@ -6043,7 +6043,7 @@
         <v>0.131586257106899</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -6078,7 +6078,7 @@
         <v>6.9014520220248898E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -6108,7 +6108,7 @@
         <v>1.7612257022159E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1">
         <v>2</v>
@@ -6141,7 +6141,7 @@
         <v>6.4995205448570903E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
@@ -6172,7 +6172,7 @@
         <v>0.110281073646743</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -6207,7 +6207,7 @@
         <v>3.5523608300555398E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -6237,7 +6237,7 @@
         <v>3.59609005036775E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1">
         <v>2</v>
@@ -6270,7 +6270,7 @@
         <v>1.8400155231055301E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
@@ -6301,7 +6301,7 @@
         <v>5.0908376710802901E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -6336,7 +6336,7 @@
         <v>8.5114844654430602E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -6366,7 +6366,7 @@
         <v>3.3373705929380403E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -6399,7 +6399,7 @@
         <v>0.118844677635465</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
@@ -6430,7 +6430,7 @@
         <v>8.0216408588473204E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
@@ -6440,7 +6440,7 @@
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
     </row>
-    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -6473,7 +6473,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
@@ -6506,7 +6506,7 @@
         <v>0.12776640253406801</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="1">
         <v>2</v>
@@ -6536,7 +6536,7 @@
         <v>0.131586257106899</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>3</v>
       </c>
@@ -6569,7 +6569,7 @@
         <v>1.7612257022159E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="1">
         <v>2</v>
@@ -6599,7 +6599,7 @@
         <v>0.110281073646743</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>4</v>
       </c>
@@ -6632,7 +6632,7 @@
         <v>3.59609005036775E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="6">
         <v>2</v>
@@ -6663,7 +6663,7 @@
         <v>5.0908376710802901E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>5</v>
       </c>
@@ -6696,7 +6696,7 @@
         <v>3.3373705929380403E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="6">
         <v>2</v>
@@ -6727,7 +6727,7 @@
         <v>8.0216408588473204E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
@@ -6737,7 +6737,7 @@
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
@@ -6747,7 +6747,7 @@
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
     </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
@@ -6757,7 +6757,7 @@
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
     </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
@@ -6767,7 +6767,7 @@
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
     </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
@@ -6777,7 +6777,7 @@
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
     </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
@@ -6787,7 +6787,7 @@
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
     </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -6797,7 +6797,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -6807,7 +6807,7 @@
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -6817,7 +6817,7 @@
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -6827,7 +6827,7 @@
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -6837,7 +6837,7 @@
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -6847,7 +6847,7 @@
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -6857,7 +6857,7 @@
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -6867,7 +6867,7 @@
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -6877,7 +6877,7 @@
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -6887,7 +6887,7 @@
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
     </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
@@ -6897,7 +6897,7 @@
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
     </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -6907,7 +6907,7 @@
       <c r="J48" s="10"/>
       <c r="K48" s="10"/>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
@@ -6917,7 +6917,7 @@
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
@@ -6927,7 +6927,7 @@
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
@@ -6937,7 +6937,7 @@
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
@@ -6947,7 +6947,7 @@
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
@@ -6973,21 +6973,21 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="78" t="s">
         <v>13</v>
       </c>
@@ -7002,8 +7002,8 @@
       <c r="J1" s="78"/>
       <c r="K1" s="78"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -7038,7 +7038,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -7073,7 +7073,7 @@
         <v>0.77960526315789502</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -7103,7 +7103,7 @@
         <v>0.95065789473684204</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1">
         <v>2</v>
@@ -7136,7 +7136,7 @@
         <v>0.83223684210526305</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
@@ -7167,7 +7167,7 @@
         <v>0.95723684210526305</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -7202,7 +7202,7 @@
         <v>0.73026315789473695</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -7232,7 +7232,7 @@
         <v>0.98684210526315796</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1">
         <v>2</v>
@@ -7265,7 +7265,7 @@
         <v>0.83552631578947401</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
@@ -7296,7 +7296,7 @@
         <v>0.98684210526315796</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -7331,7 +7331,7 @@
         <v>0.89473684210526305</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -7361,7 +7361,7 @@
         <v>0.94407894736842102</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1">
         <v>2</v>
@@ -7394,7 +7394,7 @@
         <v>0.90131578947368396</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
@@ -7425,7 +7425,7 @@
         <v>0.98026315789473695</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -7460,7 +7460,7 @@
         <v>0.94078947368421095</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -7490,7 +7490,7 @@
         <v>0.93421052631579005</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -7523,7 +7523,7 @@
         <v>0.92434210526315796</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
@@ -7554,10 +7554,10 @@
         <v>0.92105263157894701</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
     </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -7567,7 +7567,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -7577,7 +7577,7 @@
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -7587,7 +7587,7 @@
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -7597,7 +7597,7 @@
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -7607,7 +7607,7 @@
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -7617,7 +7617,7 @@
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -7627,7 +7627,7 @@
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -7637,7 +7637,7 @@
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -7647,7 +7647,7 @@
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -7657,7 +7657,7 @@
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
     </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
@@ -7667,7 +7667,7 @@
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
     </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -7677,7 +7677,7 @@
       <c r="J48" s="10"/>
       <c r="K48" s="10"/>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
@@ -7687,7 +7687,7 @@
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
@@ -7697,7 +7697,7 @@
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
@@ -7707,7 +7707,7 @@
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
@@ -7717,7 +7717,7 @@
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
@@ -7743,19 +7743,19 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.33203125" customWidth="1"/>
-    <col min="10" max="10" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="78" t="s">
         <v>18</v>
       </c>
@@ -7770,8 +7770,8 @@
       <c r="J1" s="78"/>
       <c r="K1" s="78"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -7806,7 +7806,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -7841,7 +7841,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -7871,7 +7871,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1">
         <v>2</v>
@@ -7904,7 +7904,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
@@ -7935,7 +7935,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -7970,7 +7970,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -8000,7 +8000,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1">
         <v>2</v>
@@ -8033,7 +8033,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
@@ -8064,7 +8064,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -8099,7 +8099,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -8129,7 +8129,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1">
         <v>2</v>
@@ -8162,7 +8162,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
@@ -8193,7 +8193,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -8228,7 +8228,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -8258,7 +8258,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -8291,7 +8291,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
@@ -8322,8 +8322,8 @@
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -8356,7 +8356,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
@@ -8389,7 +8389,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="1">
         <v>2</v>
@@ -8419,7 +8419,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>3</v>
       </c>
@@ -8452,7 +8452,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="1">
         <v>2</v>
@@ -8482,7 +8482,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>4</v>
       </c>
@@ -8515,7 +8515,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="6">
         <v>2</v>
@@ -8546,7 +8546,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>5</v>
       </c>
@@ -8579,7 +8579,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="6">
         <v>2</v>
@@ -8610,7 +8610,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -8620,7 +8620,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -8630,7 +8630,7 @@
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -8640,7 +8640,7 @@
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -8650,7 +8650,7 @@
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -8660,7 +8660,7 @@
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -8670,7 +8670,7 @@
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -8680,7 +8680,7 @@
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -8690,7 +8690,7 @@
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -8700,7 +8700,7 @@
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -8710,7 +8710,7 @@
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
     </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
@@ -8720,7 +8720,7 @@
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
     </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -8730,7 +8730,7 @@
       <c r="J48" s="10"/>
       <c r="K48" s="10"/>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
@@ -8740,7 +8740,7 @@
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
@@ -8750,7 +8750,7 @@
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
@@ -8760,7 +8760,7 @@
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
@@ -8770,7 +8770,7 @@
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
@@ -8796,20 +8796,20 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.44140625" customWidth="1"/>
-    <col min="10" max="10" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="78" t="s">
         <v>19</v>
       </c>
@@ -8824,8 +8824,8 @@
       <c r="J1" s="78"/>
       <c r="K1" s="78"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -8860,7 +8860,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -8895,7 +8895,7 @@
         <v>106.6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -8925,7 +8925,7 @@
         <v>160.9</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1">
         <v>2</v>
@@ -8958,7 +8958,7 @@
         <v>96.7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
@@ -8989,7 +8989,7 @@
         <v>158.9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -9024,7 +9024,7 @@
         <v>50.9</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -9054,7 +9054,7 @@
         <v>220.3</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1">
         <v>2</v>
@@ -9087,7 +9087,7 @@
         <v>95.2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
@@ -9118,7 +9118,7 @@
         <v>163.1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -9153,7 +9153,7 @@
         <v>70.099999999999994</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -9183,7 +9183,7 @@
         <v>61.6</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1">
         <v>2</v>
@@ -9216,7 +9216,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
@@ -9247,7 +9247,7 @@
         <v>53.5</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -9282,7 +9282,7 @@
         <v>193.1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -9312,7 +9312,7 @@
         <v>130.5</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -9345,7 +9345,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
@@ -9376,8 +9376,8 @@
         <v>108.3</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -9410,7 +9410,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
@@ -9443,7 +9443,7 @@
         <v>160.9</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="1">
         <v>2</v>
@@ -9473,7 +9473,7 @@
         <v>158.9</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>3</v>
       </c>
@@ -9506,7 +9506,7 @@
         <v>220.3</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="1">
         <v>2</v>
@@ -9536,7 +9536,7 @@
         <v>163.1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>4</v>
       </c>
@@ -9569,7 +9569,7 @@
         <v>61.6</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="6">
         <v>2</v>
@@ -9600,7 +9600,7 @@
         <v>53.5</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>5</v>
       </c>
@@ -9633,7 +9633,7 @@
         <v>130.5</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="6">
         <v>2</v>
@@ -9664,7 +9664,7 @@
         <v>108.3</v>
       </c>
     </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -9674,7 +9674,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -9684,7 +9684,7 @@
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -9694,7 +9694,7 @@
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -9704,7 +9704,7 @@
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -9714,7 +9714,7 @@
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -9724,7 +9724,7 @@
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -9734,7 +9734,7 @@
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -9744,7 +9744,7 @@
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -9754,7 +9754,7 @@
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -9764,7 +9764,7 @@
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
     </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
@@ -9774,7 +9774,7 @@
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
     </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -9784,7 +9784,7 @@
       <c r="J48" s="10"/>
       <c r="K48" s="10"/>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
@@ -9794,7 +9794,7 @@
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
@@ -9804,7 +9804,7 @@
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
@@ -9814,7 +9814,7 @@
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
@@ -9824,7 +9824,7 @@
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
@@ -9850,22 +9850,22 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.21875" customWidth="1"/>
-    <col min="11" max="11" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="78" t="s">
         <v>20</v>
       </c>
@@ -9880,8 +9880,8 @@
       <c r="J1" s="78"/>
       <c r="K1" s="78"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -9916,7 +9916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -9951,7 +9951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -9981,7 +9981,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1">
         <v>2</v>
@@ -10014,7 +10014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
@@ -10045,7 +10045,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -10080,7 +10080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -10110,7 +10110,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1">
         <v>2</v>
@@ -10143,7 +10143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
@@ -10174,7 +10174,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -10209,7 +10209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -10239,7 +10239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1">
         <v>2</v>
@@ -10272,7 +10272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
@@ -10303,7 +10303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -10338,7 +10338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -10368,7 +10368,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -10401,7 +10401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
@@ -10432,8 +10432,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -10466,7 +10466,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
@@ -10499,7 +10499,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="1">
         <v>2</v>
@@ -10529,7 +10529,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>3</v>
       </c>
@@ -10562,7 +10562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="1">
         <v>2</v>
@@ -10592,7 +10592,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>4</v>
       </c>
@@ -10625,7 +10625,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="6">
         <v>2</v>
@@ -10656,7 +10656,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>5</v>
       </c>
@@ -10689,7 +10689,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="6">
         <v>2</v>
@@ -10720,7 +10720,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -10730,7 +10730,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -10740,7 +10740,7 @@
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -10750,7 +10750,7 @@
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -10760,7 +10760,7 @@
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -10770,7 +10770,7 @@
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -10780,7 +10780,7 @@
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -10790,7 +10790,7 @@
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -10800,7 +10800,7 @@
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -10810,7 +10810,7 @@
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -10820,7 +10820,7 @@
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
     </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
@@ -10830,7 +10830,7 @@
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
     </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -10840,7 +10840,7 @@
       <c r="J48" s="10"/>
       <c r="K48" s="10"/>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
@@ -10850,7 +10850,7 @@
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
@@ -10860,7 +10860,7 @@
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
@@ -10870,7 +10870,7 @@
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
@@ -10880,7 +10880,7 @@
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
@@ -10906,21 +10906,21 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="78" t="s">
         <v>21</v>
       </c>
@@ -10935,8 +10935,8 @@
       <c r="J1" s="78"/>
       <c r="K1" s="78"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -10971,7 +10971,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -11006,7 +11006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -11036,7 +11036,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1">
         <v>2</v>
@@ -11069,7 +11069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
@@ -11100,7 +11100,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -11135,7 +11135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -11165,7 +11165,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1">
         <v>2</v>
@@ -11198,7 +11198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
@@ -11229,7 +11229,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -11264,7 +11264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -11294,7 +11294,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1">
         <v>2</v>
@@ -11327,7 +11327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
@@ -11358,7 +11358,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -11393,7 +11393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -11423,7 +11423,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -11456,7 +11456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
@@ -11487,8 +11487,8 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -11521,7 +11521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
@@ -11554,7 +11554,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="1">
         <v>2</v>
@@ -11584,7 +11584,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>3</v>
       </c>
@@ -11617,7 +11617,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="1">
         <v>2</v>
@@ -11647,7 +11647,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>4</v>
       </c>
@@ -11680,7 +11680,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="6">
         <v>2</v>
@@ -11711,7 +11711,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>5</v>
       </c>
@@ -11744,7 +11744,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="6">
         <v>2</v>
@@ -11775,7 +11775,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -11785,7 +11785,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -11795,7 +11795,7 @@
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -11805,7 +11805,7 @@
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -11815,7 +11815,7 @@
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -11825,7 +11825,7 @@
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -11835,7 +11835,7 @@
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -11845,7 +11845,7 @@
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -11855,7 +11855,7 @@
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -11865,7 +11865,7 @@
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -11875,7 +11875,7 @@
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
     </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
@@ -11885,7 +11885,7 @@
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
     </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -11895,7 +11895,7 @@
       <c r="J48" s="10"/>
       <c r="K48" s="10"/>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
@@ -11905,7 +11905,7 @@
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
@@ -11915,7 +11915,7 @@
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
@@ -11925,7 +11925,7 @@
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
@@ -11935,7 +11935,7 @@
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
@@ -11961,26 +11961,26 @@
       <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.44140625" customWidth="1"/>
-    <col min="15" max="15" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.42578125" customWidth="1"/>
+    <col min="15" max="15" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="78" t="s">
         <v>26</v>
       </c>
@@ -12000,8 +12000,8 @@
       <c r="O1" s="78"/>
       <c r="P1" s="78"/>
     </row>
-    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="13" t="s">
         <v>6</v>
       </c>
@@ -12032,7 +12032,7 @@
       </c>
       <c r="P3" s="82"/>
     </row>
-    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -12082,7 +12082,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -12132,7 +12132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="17" t="s">
         <v>12</v>
@@ -12177,7 +12177,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1">
         <v>2</v>
@@ -12225,7 +12225,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="18" t="s">
@@ -12271,7 +12271,7 @@
         <v>1.5625E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -12321,7 +12321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="17" t="s">
         <v>12</v>
@@ -12366,7 +12366,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1">
         <v>2</v>
@@ -12414,7 +12414,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="18" t="s">
@@ -12460,7 +12460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -12510,7 +12510,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="17" t="s">
         <v>12</v>
@@ -12555,7 +12555,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1">
         <v>2</v>
@@ -12603,7 +12603,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="18" t="s">
@@ -12649,7 +12649,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -12699,7 +12699,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="17" t="s">
         <v>12</v>
@@ -12744,7 +12744,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -12792,7 +12792,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="18" t="s">
@@ -12838,10 +12838,10 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
     </row>
-    <row r="37" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -12855,7 +12855,7 @@
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
     </row>
-    <row r="38" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -12869,7 +12869,7 @@
       <c r="N38" s="10"/>
       <c r="O38" s="10"/>
     </row>
-    <row r="39" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -12883,7 +12883,7 @@
       <c r="N39" s="10"/>
       <c r="O39" s="10"/>
     </row>
-    <row r="40" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -12897,7 +12897,7 @@
       <c r="N40" s="10"/>
       <c r="O40" s="10"/>
     </row>
-    <row r="41" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -12911,7 +12911,7 @@
       <c r="N41" s="10"/>
       <c r="O41" s="10"/>
     </row>
-    <row r="42" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -12925,7 +12925,7 @@
       <c r="N42" s="10"/>
       <c r="O42" s="10"/>
     </row>
-    <row r="43" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -12939,7 +12939,7 @@
       <c r="N43" s="10"/>
       <c r="O43" s="10"/>
     </row>
-    <row r="44" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -12953,7 +12953,7 @@
       <c r="N44" s="10"/>
       <c r="O44" s="10"/>
     </row>
-    <row r="45" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -12967,7 +12967,7 @@
       <c r="N45" s="10"/>
       <c r="O45" s="10"/>
     </row>
-    <row r="46" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -12981,7 +12981,7 @@
       <c r="N46" s="10"/>
       <c r="O46" s="10"/>
     </row>
-    <row r="47" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
@@ -12995,7 +12995,7 @@
       <c r="N47" s="10"/>
       <c r="O47" s="10"/>
     </row>
-    <row r="48" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -13009,7 +13009,7 @@
       <c r="N48" s="10"/>
       <c r="O48" s="10"/>
     </row>
-    <row r="49" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
@@ -13023,7 +13023,7 @@
       <c r="N49" s="10"/>
       <c r="O49" s="10"/>
     </row>
-    <row r="50" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
@@ -13037,7 +13037,7 @@
       <c r="N50" s="10"/>
       <c r="O50" s="10"/>
     </row>
-    <row r="51" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
@@ -13051,7 +13051,7 @@
       <c r="N51" s="10"/>
       <c r="O51" s="10"/>
     </row>
-    <row r="52" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
@@ -13065,7 +13065,7 @@
       <c r="N52" s="10"/>
       <c r="O52" s="10"/>
     </row>
-    <row r="53" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>

</xml_diff>